<commit_message>
added posts for final yr and executive member post for all others added hult posters just for fun
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="72">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">First</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorem De coutij</t>
+    <t xml:space="preserve">Volunteer</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/ligmitz</t>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Second</t>
   </si>
   <si>
+    <t xml:space="preserve">Executive Member</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kunal Thakur</t>
   </si>
   <si>
@@ -154,46 +157,88 @@
     <t xml:space="preserve">Final</t>
   </si>
   <si>
+    <t xml:space="preserve">President</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marmik Sharma</t>
   </si>
   <si>
+    <t xml:space="preserve">Technical Secetary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mayank Singh</t>
   </si>
   <si>
+    <t xml:space="preserve">Vice President</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mukul C. Mahadik</t>
   </si>
   <si>
+    <t xml:space="preserve">Joint Secretary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sumit Sharma</t>
   </si>
   <si>
+    <t xml:space="preserve">Finance Secretary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abhiraj Singh Rathore</t>
   </si>
   <si>
+    <t xml:space="preserve">Marketing Head</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amol Bobade</t>
   </si>
   <si>
+    <t xml:space="preserve">Joint Finance Secretary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Divyanshu Bhaik</t>
   </si>
   <si>
+    <t xml:space="preserve">Joint Technical Secretary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kunal Kishore</t>
   </si>
   <si>
+    <t xml:space="preserve">Media Head</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sahaj Kulshrestha</t>
   </si>
   <si>
+    <t xml:space="preserve">Creative Head</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parthivi Jain</t>
   </si>
   <si>
+    <t xml:space="preserve">PR Head</t>
+  </si>
+  <si>
     <t xml:space="preserve">Varan Singh Rohila</t>
   </si>
   <si>
     <t xml:space="preserve">Achyut Sharma</t>
   </si>
   <si>
+    <t xml:space="preserve">Orgi Head</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priyanka </t>
   </si>
   <si>
+    <t xml:space="preserve">Design Head</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rishi Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretary</t>
   </si>
 </sst>
 </file>
@@ -323,17 +368,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
   </cols>
@@ -527,17 +572,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
@@ -570,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -581,13 +626,13 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -598,13 +643,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -615,13 +660,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -632,13 +677,13 @@
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -649,13 +694,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -666,13 +711,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -683,13 +728,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -700,13 +745,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -717,13 +762,13 @@
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -734,13 +779,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -751,13 +796,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -768,13 +813,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -785,13 +830,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -838,17 +883,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
@@ -874,13 +919,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -891,13 +936,13 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -908,13 +953,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -925,13 +970,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -942,13 +987,13 @@
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -959,13 +1004,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -976,13 +1021,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -993,13 +1038,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -1010,13 +1055,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -1027,13 +1072,13 @@
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -1044,13 +1089,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -1061,13 +1106,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1078,13 +1123,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1095,13 +1140,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -1112,13 +1157,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1162,17 +1207,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>
@@ -1198,13 +1243,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -1215,13 +1260,13 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -1232,13 +1277,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -1249,13 +1294,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -1266,13 +1311,13 @@
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -1283,13 +1328,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -1300,13 +1345,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -1317,13 +1362,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -1334,13 +1379,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -1351,13 +1396,13 @@
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -1368,13 +1413,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -1385,13 +1430,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1402,13 +1447,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1419,13 +1464,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -1436,13 +1481,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
members: Update members page information.
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="102">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -160,85 +160,175 @@
     <t xml:space="preserve">President</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/vivek-gusain-656b78157/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/vivek.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marmik Sharma</t>
   </si>
   <si>
     <t xml:space="preserve">Technical Secetary</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/marmik07/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/marmik.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mayank Singh</t>
   </si>
   <si>
     <t xml:space="preserve">Vice President</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/dyknoww/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/mayank.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mukul C. Mahadik</t>
   </si>
   <si>
     <t xml:space="preserve">Joint Secretary</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/mukulm03/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/mukul.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sumit Sharma</t>
   </si>
   <si>
     <t xml:space="preserve">Finance Secretary</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/sumit-sharma-a54814181/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/sumit.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abhiraj Singh Rathore</t>
   </si>
   <si>
     <t xml:space="preserve">Marketing Head</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/abhiraj-singh-rathore-170499/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/abhiraj.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amol Bobade</t>
   </si>
   <si>
     <t xml:space="preserve">Joint Finance Secretary</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/amol-bobade-97b34b179/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/amol.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Divyanshu Bhaik</t>
   </si>
   <si>
     <t xml:space="preserve">Joint Technical Secretary</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/divyanshu-bhaik-7438a6155/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/divyanshu.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kunal Kishore</t>
   </si>
   <si>
     <t xml:space="preserve">Media Head</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/kunal-kishore-79742814b/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/kunal.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sahaj Kulshrestha</t>
   </si>
   <si>
     <t xml:space="preserve">Creative Head</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/sahaj-kulshrestha/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/sahaj.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parthivi Jain</t>
   </si>
   <si>
     <t xml:space="preserve">PR Head</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/parthivi-jain/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/parthivi.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Varan Singh Rohila</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/varan-singh-rohila/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/varan.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Achyut Sharma</t>
   </si>
   <si>
     <t xml:space="preserve">Orgi Head</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/achyut-sharma-7508a0b4/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/achyut.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priyanka </t>
   </si>
   <si>
     <t xml:space="preserve">Design Head</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/priyanka-kumar-a1135a1a1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/priyanka.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rishi Kumar</t>
   </si>
   <si>
     <t xml:space="preserve">Secretary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/rishi-kumar-5b808b153/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/rishi.jpg</t>
   </si>
 </sst>
 </file>
@@ -374,11 +464,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
   </cols>
@@ -582,7 +672,7 @@
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
@@ -893,7 +983,7 @@
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
@@ -1213,11 +1303,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>
@@ -1241,7 +1331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -1252,248 +1342,248 @@
         <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,21 +1593,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D16" r:id="rId15" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D4" r:id="rId1" display="https://www.linkedin.com/in/dyknoww/"/>
+    <hyperlink ref="D6" r:id="rId2" display="https://www.linkedin.com/in/sumit-sharma-a54814181/"/>
+    <hyperlink ref="D7" r:id="rId3" display="https://www.linkedin.com/in/abhiraj-singh-rathore-170499/"/>
+    <hyperlink ref="D8" r:id="rId4" display="https://www.linkedin.com/in/amol-bobade-97b34b179/"/>
+    <hyperlink ref="D9" r:id="rId5" display="https://www.linkedin.com/in/divyanshu-bhaik-7438a6155/"/>
+    <hyperlink ref="D10" r:id="rId6" display="https://www.linkedin.com/in/kunal-kishore-79742814b/"/>
+    <hyperlink ref="D13" r:id="rId7" display="https://www.linkedin.com/in/varan-singh-rohila/"/>
+    <hyperlink ref="D14" r:id="rId8" display="https://www.linkedin.com/in/achyut-sharma-7508a0b4/"/>
+    <hyperlink ref="D15" r:id="rId9" display="https://www.linkedin.com/in/priyanka-kumar-a1135a1a1/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
members: Update information and pictures.
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="156">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -64,91 +64,253 @@
     <t xml:space="preserve">Executive Member</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/gaurav-pandey-412180194/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/gaurav.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kunal Thakur</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/kunal-thakur-b27823193/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/kunalt.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ayushi Sharma</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/ayushi-sharma-778657198/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/ayushi.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jai Gupta</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/jai-gupta-8b5238196/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/jai.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manvendra Singh Chauhan</t>
   </si>
   <si>
-    <t xml:space="preserve">Mayur Singh</t>
+    <t xml:space="preserve">https://www.instagram.com/mnvndra/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/manvendra.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayur Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/mayur-kumar-47a9511a1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/mayur.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Paras Aggarwal</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/parasaggarwal/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/paras.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parth Pant</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/parth-pant-866bb4189/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/parth.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rahul Kumar</t>
   </si>
   <si>
     <t xml:space="preserve">Suryansh Dwivedi</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/suryansh-dwivedi-9b9975199/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/suryansh.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Utkarsh Rai</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/utkarsh-rai-50738b61/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/utkarsh.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Uditee Singh</t>
   </si>
   <si>
     <t xml:space="preserve">Vanshika Thakur</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/vanshika-thakur-6a7b4a19a/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/vanshika.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vasundhra Thakur</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/vasundhra-thakur-5b9023196/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/vasundhra.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yash Punia</t>
   </si>
   <si>
     <t xml:space="preserve">Third</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/yash-punia/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/yash.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aakhya Rai</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/akhyarai/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/akhya.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abhay Raj Singh Rathod</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/rathod-sahaab/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/abhay.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aditi Singh</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/aditi-singh2000/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/aditi.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anshudhar Kumar Singh</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/anshudhar-kumar-singh/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/anshudhar.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arsh Sharma</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/sov-trotter/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/arsh.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Harshit Srivastav</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/harshit-srivastav-1507/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/harshit.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nimish Lata</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/nimish-sharma-0b0929195/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/nimish.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rohan Nawathe</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/rnawathe/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/rohan.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sarvesh Srivastav</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/sarvesh-srivastava-03678116b/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/sarvesh.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tanuja Pal</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.facebook.com/tanuja.pal.75436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/tanuja.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tanya Bhandari</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/tanyabhandari25/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/tanya.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anika Sharma</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/sharma3anika/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/anika.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ajay Chahar</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/ajay-c-200a9b110/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/ajay.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vishal Dhiman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/vishal-dhiman-b99a9b18b/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../members/vishal.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Vivek Gussain</t>
@@ -468,7 +630,7 @@
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
   </cols>
@@ -668,11 +830,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
@@ -708,15 +870,15 @@
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -725,15 +887,15 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -742,15 +904,15 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -759,15 +921,15 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -776,15 +938,15 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -793,15 +955,15 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -810,15 +972,15 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -827,15 +989,15 @@
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -850,9 +1012,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -861,15 +1023,15 @@
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -878,15 +1040,15 @@
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -895,15 +1057,15 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -912,15 +1074,15 @@
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -929,10 +1091,10 @@
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,20 +1109,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://www.linkedin.com/in/gaurav-pandey-412180194/"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://www.linkedin.com/in/kunal-thakur-b27823193/"/>
+    <hyperlink ref="D7" r:id="rId3" display="https://www.linkedin.com/in/mayur-kumar-47a9511a1/"/>
+    <hyperlink ref="D8" r:id="rId4" display="https://www.linkedin.com/in/parasaggarwal/"/>
+    <hyperlink ref="D9" r:id="rId5" display="https://www.linkedin.com/in/parth-pant-866bb4189/"/>
+    <hyperlink ref="D10" r:id="rId6" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D13" r:id="rId7" display="https://www.linkedin.com/in/suryansh-dwivedi-9b9975199/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -980,10 +1135,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
@@ -1007,259 +1162,259 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,21 +1425,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://github.com/ligmitz"/>
-    <hyperlink ref="D16" r:id="rId15" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D4" r:id="rId1" display="https://www.linkedin.com/in/rathod-sahaab/"/>
+    <hyperlink ref="D5" r:id="rId2" display="https://www.linkedin.com/in/aditi-singh2000/"/>
+    <hyperlink ref="D7" r:id="rId3" display="https://www.linkedin.com/in/sov-trotter/"/>
+    <hyperlink ref="D8" r:id="rId4" display="https://www.linkedin.com/in/harshit-srivastav-1507/"/>
+    <hyperlink ref="D10" r:id="rId5" display="https://www.linkedin.com/in/rnawathe/"/>
+    <hyperlink ref="D11" r:id="rId6" display="https://www.linkedin.com/in/sarvesh-srivastava-03678116b/"/>
+    <hyperlink ref="D14" r:id="rId7" display="https://www.linkedin.com/in/sharma3anika/"/>
+    <hyperlink ref="D16" r:id="rId8" display="https://www.linkedin.com/in/vishal-dhiman-b99a9b18b/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1303,11 +1451,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>
@@ -1333,257 +1481,257 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix: Adding image and typo correction.
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="157">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -157,6 +157,9 @@
     <t xml:space="preserve">Uditee Singh</t>
   </si>
   <si>
+    <t xml:space="preserve">../members/uditee.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vanshika Thakur</t>
   </si>
   <si>
@@ -259,7 +262,7 @@
     <t xml:space="preserve">../members/rohan.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarvesh Srivastav</t>
+    <t xml:space="preserve">Sarvesh Srivastava</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.linkedin.com/in/sarvesh-srivastava-03678116b/</t>
@@ -630,7 +633,7 @@
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
   </cols>
@@ -831,10 +834,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
@@ -1060,12 +1063,12 @@
         <v>38</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -1074,15 +1077,15 @@
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -1091,10 +1094,10 @@
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,10 +1138,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
@@ -1164,257 +1167,257 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,7 +1458,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>
@@ -1481,257 +1484,257 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
typo: fix typo in members sheet.
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">Third</t>
   </si>
   <si>
-    <t xml:space="preserve">Coordinatior</t>
+    <t xml:space="preserve">Coordinator</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.linkedin.com/in/yash-punia/</t>
@@ -358,7 +358,7 @@
     <t xml:space="preserve">Marmik Sharma</t>
   </si>
   <si>
-    <t xml:space="preserve">Technical Secetary</t>
+    <t xml:space="preserve">Technical Secretary</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.linkedin.com/in/marmik07/</t>
@@ -657,7 +657,7 @@
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
   </cols>
@@ -861,7 +861,7 @@
       <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
@@ -1188,11 +1188,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
@@ -1505,11 +1505,11 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>

</xml_diff>

<commit_message>
added first year to members page
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\istenith.github.io\content\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Web-Application\istenith.github.io\content\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D617F8D-F6EC-4074-864E-6B1C8F3DB0E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A751F6A-490F-4EE9-A572-25C21389383E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="202">
   <si>
     <t>name</t>
   </si>
@@ -45,21 +45,12 @@
     <t>img</t>
   </si>
   <si>
-    <t>Binod</t>
-  </si>
-  <si>
     <t>First</t>
   </si>
   <si>
     <t>Volunteer</t>
   </si>
   <si>
-    <t>https://github.com/ligmitz</t>
-  </si>
-  <si>
-    <t>../members/balidaan.jpg</t>
-  </si>
-  <si>
     <t>Gaurav Pandey</t>
   </si>
   <si>
@@ -529,6 +520,120 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/uditee-singh-7619921b0/</t>
+  </si>
+  <si>
+    <t>Albert Sharma</t>
+  </si>
+  <si>
+    <t>Deepak Singh</t>
+  </si>
+  <si>
+    <t>Dev Khanduja</t>
+  </si>
+  <si>
+    <t>Divyansh Tripathi</t>
+  </si>
+  <si>
+    <t>Gazal Shyam</t>
+  </si>
+  <si>
+    <t>Harmanpreet Singh</t>
+  </si>
+  <si>
+    <t>Harshwardhan Fartale</t>
+  </si>
+  <si>
+    <t>Kartik</t>
+  </si>
+  <si>
+    <t>Kaustubh Verma</t>
+  </si>
+  <si>
+    <t>Lovkesh Bansal</t>
+  </si>
+  <si>
+    <t>Mayank Thakur</t>
+  </si>
+  <si>
+    <t>Meenakshi</t>
+  </si>
+  <si>
+    <t>Noel Kankipati</t>
+  </si>
+  <si>
+    <t>Sheetanshu Shreeyansh</t>
+  </si>
+  <si>
+    <t>Shriya Chauhan</t>
+  </si>
+  <si>
+    <t>Shruti Bhatia</t>
+  </si>
+  <si>
+    <t>Sumit Dhiman</t>
+  </si>
+  <si>
+    <t>Vansh Thakur</t>
+  </si>
+  <si>
+    <t>Vanshika Sood</t>
+  </si>
+  <si>
+    <t>../members/Albert.jpg</t>
+  </si>
+  <si>
+    <t>../members/Deepak.jpg</t>
+  </si>
+  <si>
+    <t>../members/Dev.jpg</t>
+  </si>
+  <si>
+    <t>../members/Gazal.jpg</t>
+  </si>
+  <si>
+    <t>../members/Harmanpreet.jpg</t>
+  </si>
+  <si>
+    <t>../members/Harshwardhan.jpg</t>
+  </si>
+  <si>
+    <t>../members/Kartik.jpg</t>
+  </si>
+  <si>
+    <t>../members/Divyansh.jpeg</t>
+  </si>
+  <si>
+    <t>../members/Kaustubh.jpg</t>
+  </si>
+  <si>
+    <t>../members/Lovekesh.jpeg</t>
+  </si>
+  <si>
+    <t>../members/Mayank2.jpg</t>
+  </si>
+  <si>
+    <t>../members/Meenakshi.jpg</t>
+  </si>
+  <si>
+    <t>../members/noel.jpeg</t>
+  </si>
+  <si>
+    <t>../members/Sheetanshu.jpg</t>
+  </si>
+  <si>
+    <t>../members/shriya.jpg</t>
+  </si>
+  <si>
+    <t>../members/Shruti.jpg</t>
+  </si>
+  <si>
+    <t>../members/Sumit2.jpg</t>
+  </si>
+  <si>
+    <t>../members/Vansh.jpg</t>
+  </si>
+  <si>
+    <t>../members/Vanshika2.jpg</t>
   </si>
 </sst>
 </file>
@@ -912,14 +1017,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -942,164 +1048,331 @@
     </row>
     <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
+      <c r="D2" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
+      <c r="D3" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
+      <c r="D4" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
+      <c r="D5" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
+      <c r="D6" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
+      <c r="D7" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D3:D20" r:id="rId2" display="https://www.istenith.com/" xr:uid="{63CCF2C6-B0C7-4F21-BAE7-B0AD4A66A001}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1110,7 +1383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1141,274 +1414,274 @@
     </row>
     <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
@@ -1467,257 +1740,257 @@
     </row>
     <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
@@ -1780,257 +2053,257 @@
     </row>
     <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
corrected photo on sumit
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Web-Application\istenith.github.io\content\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A751F6A-490F-4EE9-A572-25C21389383E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035DBB8C-BEC9-473D-AD94-44D964FCF4C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,13 +627,13 @@
     <t>../members/Shruti.jpg</t>
   </si>
   <si>
-    <t>../members/Sumit2.jpg</t>
-  </si>
-  <si>
     <t>../members/Vansh.jpg</t>
   </si>
   <si>
     <t>../members/Vanshika2.jpg</t>
+  </si>
+  <si>
+    <t>../members/Sumit2.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1332,7 @@
         <v>162</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>162</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
         <v>162</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maintainance: remove phantom and add posters
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="202">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -161,15 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">../members/Vanshika2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phantom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://docs.google.com/document/d/1XFpuAsdo34SlYNS2PZj3x3o9s1D9l3mGLicVJs0q6MM/edit?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/phantom.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Gaurav Pandey</t>
@@ -744,7 +735,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -766,10 +757,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -851,13 +838,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.22"/>
@@ -1203,25 +1190,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://www.istenith.com/"/>
@@ -1243,7 +1214,6 @@
     <hyperlink ref="D18" r:id="rId17" display="https://www.istenith.com/"/>
     <hyperlink ref="D19" r:id="rId18" display="https://www.istenith.com/"/>
     <hyperlink ref="D20" r:id="rId19" display="https://www.istenith.com/"/>
-    <hyperlink ref="D21" r:id="rId20" display="https://docs.google.com/document/d/1XFpuAsdo34SlYNS2PZj3x3o9s1D9l3mGLicVJs0q6MM/edit?usp=sharing"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1266,7 +1236,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.56"/>
@@ -1293,274 +1263,274 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,7 +1567,7 @@
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
@@ -1623,257 +1593,257 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,11 +1884,11 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,257 +1910,257 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
edited Members images and Members.xls
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumit Dhiman\OneDrive\Documents\istenith.github.io\content\sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3A999DCE-5727-443F-9E52-8EC9F3FB2E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Sumit Dhiman - Personal View" guid="{DF53FF45-CD95-46C9-A254-8606AC4BE6BE}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1048" tabRatio="500" activeSheetId="2"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -23,553 +31,553 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="168">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albert Sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.istenith.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Albert.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deepak Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Deepak.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dev Khanduja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Dev.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divyansh Tripathi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Divyansh.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gazal Shyam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Gazal.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harmanpreet Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Harmanpreet.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harshwardhan Fartale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Harshwardhan.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kartik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Kartik.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaustubh Verma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Kaustubh.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lovkesh Bansal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Lovekesh.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mayank Thakur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Mayank2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meenakshi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Meenakshi.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noel Kankipati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/noel.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheetanshu Shreeyansh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Sheetanshu.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shriya Chauhan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/shriya.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shruti Bhatia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Shruti.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumit Dhiman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Sumit2.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vansh Thakur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Vansh.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanshika Sood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/Vanshika2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Executive Member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/albert-sharma-2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/deepak-singh-a04ba51ba/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/dev-khanduja/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/divyansh-tripathi-4bb66a205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/kartik-576b24205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/vermakaustubh28/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/lovekesh-bansal-123786191</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/meenakshi-33b683205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/noel-kankipati-444b1a217/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/shriya-chauhan-20a19b200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/sumit-dhiman-20bce091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/vansh-thakur-b029a4202/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaurav Pandey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/gaurav-pandey-412180194/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/gaurav.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kunal Thakur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/kunal-thakur-b27823193/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/kunalt.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ayushi Sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/ayushi-sharma-778657198/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/ayushi.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jai Gupta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/jai-gupta-8b5238196/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/jai.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manvendra Singh Chauhan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.instagram.com/mnvndra/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/manvendra.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mayur Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/mayur-kumar-47a9511a1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/mayur.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paras Aggarwal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/parasaggarwal/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/paras.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parth Pant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/parth-pant-866bb4189/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/parth.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rahul Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/na.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suryansh Dwivedi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/suryansh-dwivedi-9b9975199/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/suryansh.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utkarsh Rai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/utkarsh-rai-50738b61/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/utkarsh.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uditee Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/uditee-singh-7619921b0/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/uditee.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanshika Thakur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/vanshika-thakur-6a7b4a19a/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/vanshika.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vasundhra Thakur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/vasundhra-thakur-5b9023196/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/vasundhra.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaurav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/gaurav-2b5a73195/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/gaurav2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pragya Angra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/pragya-angra-3a87421a9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/pragya.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yash Punia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">President</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/yash-punia/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/yash.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akhya Rai</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="175">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>Albert Sharma</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>https://www.istenith.com/</t>
+  </si>
+  <si>
+    <t>../members/Albert.jpg</t>
+  </si>
+  <si>
+    <t>Deepak Singh</t>
+  </si>
+  <si>
+    <t>../members/Deepak.jpg</t>
+  </si>
+  <si>
+    <t>Dev Khanduja</t>
+  </si>
+  <si>
+    <t>../members/Dev.jpg</t>
+  </si>
+  <si>
+    <t>Divyansh Tripathi</t>
+  </si>
+  <si>
+    <t>../members/Divyansh.jpeg</t>
+  </si>
+  <si>
+    <t>Gazal Shyam</t>
+  </si>
+  <si>
+    <t>../members/Gazal.jpg</t>
+  </si>
+  <si>
+    <t>Harmanpreet Singh</t>
+  </si>
+  <si>
+    <t>../members/Harmanpreet.jpg</t>
+  </si>
+  <si>
+    <t>Harshwardhan Fartale</t>
+  </si>
+  <si>
+    <t>../members/Harshwardhan.jpg</t>
+  </si>
+  <si>
+    <t>Kartik</t>
+  </si>
+  <si>
+    <t>../members/Kartik.jpg</t>
+  </si>
+  <si>
+    <t>Kaustubh Verma</t>
+  </si>
+  <si>
+    <t>../members/Kaustubh.jpg</t>
+  </si>
+  <si>
+    <t>Lovkesh Bansal</t>
+  </si>
+  <si>
+    <t>../members/Lovekesh.jpeg</t>
+  </si>
+  <si>
+    <t>Mayank Thakur</t>
+  </si>
+  <si>
+    <t>../members/Mayank2.jpg</t>
+  </si>
+  <si>
+    <t>Meenakshi</t>
+  </si>
+  <si>
+    <t>../members/Meenakshi.jpg</t>
+  </si>
+  <si>
+    <t>Noel Kankipati</t>
+  </si>
+  <si>
+    <t>../members/noel.jpeg</t>
+  </si>
+  <si>
+    <t>Sheetanshu Shreeyansh</t>
+  </si>
+  <si>
+    <t>../members/Sheetanshu.jpg</t>
+  </si>
+  <si>
+    <t>Shriya Chauhan</t>
+  </si>
+  <si>
+    <t>../members/shriya.jpg</t>
+  </si>
+  <si>
+    <t>Shruti Bhatia</t>
+  </si>
+  <si>
+    <t>../members/Shruti.jpg</t>
+  </si>
+  <si>
+    <t>Sumit Dhiman</t>
+  </si>
+  <si>
+    <t>../members/Sumit2.jpeg</t>
+  </si>
+  <si>
+    <t>Vansh Thakur</t>
+  </si>
+  <si>
+    <t>../members/Vansh.jpg</t>
+  </si>
+  <si>
+    <t>Vanshika Sood</t>
+  </si>
+  <si>
+    <t>../members/Vanshika2.jpg</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Executive Member</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/albert-sharma-2016</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/deepak-singh-a04ba51ba/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dev-khanduja/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/divyansh-tripathi-4bb66a205</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kartik-576b24205</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vermakaustubh28/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/meenakshi-33b683205</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/noel-kankipati-444b1a217/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shriya-chauhan-20a19b200</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sumit-dhiman-20bce091</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vansh-thakur-b029a4202/</t>
+  </si>
+  <si>
+    <t>Gaurav Pandey</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Coordinator</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/gaurav-pandey-412180194/</t>
+  </si>
+  <si>
+    <t>../members/gaurav.jpg</t>
+  </si>
+  <si>
+    <t>Kunal Thakur</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kunal-thakur-b27823193/</t>
+  </si>
+  <si>
+    <t>../members/kunalt.jpg</t>
+  </si>
+  <si>
+    <t>Ayushi Sharma</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ayushi-sharma-778657198/</t>
+  </si>
+  <si>
+    <t>../members/ayushi.jpg</t>
+  </si>
+  <si>
+    <t>Jai Gupta</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jai-gupta-8b5238196/</t>
+  </si>
+  <si>
+    <t>../members/jai.jpg</t>
+  </si>
+  <si>
+    <t>Manvendra Singh Chauhan</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/mnvndra/</t>
+  </si>
+  <si>
+    <t>../members/manvendra.jpg</t>
+  </si>
+  <si>
+    <t>Mayur Kumar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/mayur-kumar-47a9511a1/</t>
+  </si>
+  <si>
+    <t>../members/mayur.jpg</t>
+  </si>
+  <si>
+    <t>Paras Aggarwal</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/parasaggarwal/</t>
+  </si>
+  <si>
+    <t>../members/paras.jpg</t>
+  </si>
+  <si>
+    <t>Parth Pant</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/parth-pant-866bb4189/</t>
+  </si>
+  <si>
+    <t>../members/parth.jpg</t>
+  </si>
+  <si>
+    <t>Rahul Kumar</t>
+  </si>
+  <si>
+    <t>../members/na.jpg</t>
+  </si>
+  <si>
+    <t>Suryansh Dwivedi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/suryansh-dwivedi-9b9975199/</t>
+  </si>
+  <si>
+    <t>../members/suryansh.jpg</t>
+  </si>
+  <si>
+    <t>Utkarsh Rai</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/utkarsh-rai-50738b61/</t>
+  </si>
+  <si>
+    <t>../members/utkarsh.jpg</t>
+  </si>
+  <si>
+    <t>Uditee Singh</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/uditee-singh-7619921b0/</t>
+  </si>
+  <si>
+    <t>../members/uditee.jpg</t>
+  </si>
+  <si>
+    <t>Vanshika Thakur</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vanshika-thakur-6a7b4a19a/</t>
+  </si>
+  <si>
+    <t>../members/vanshika.jpg</t>
+  </si>
+  <si>
+    <t>Vasundhra Thakur</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vasundhra-thakur-5b9023196/</t>
+  </si>
+  <si>
+    <t>../members/vasundhra.jpg</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/gaurav-2b5a73195/</t>
+  </si>
+  <si>
+    <t>../members/gaurav2.jpg</t>
+  </si>
+  <si>
+    <t>Pragya Angra</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/pragya-angra-3a87421a9/</t>
+  </si>
+  <si>
+    <t>../members/pragya.jpg</t>
+  </si>
+  <si>
+    <t>Yash Punia</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/yash-punia/</t>
+  </si>
+  <si>
+    <t>../members/yash.jpg</t>
+  </si>
+  <si>
+    <t>Akhya Rai</t>
   </si>
   <si>
     <t xml:space="preserve">Joint Secretary </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/akhyarai/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/akhya.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abhay Raj Singh Rathod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joint Technical Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/rathod-sahaab/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/abhay.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aditi Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/aditi-singh2000/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/aditi.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anshudhar Kumar Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/anshudhar-kumar-singh/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/anshudhar.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arsh Sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/sov-trotter/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/arsh.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harshit Srivastav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/harshit-srivastav-1507/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/harshit.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nimish Lata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/nimish-sharma-0b0929195/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/nimish.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohan Nawathe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/rnawathe/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/rohan.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarvesh Srivastava</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vice President</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/sarvesh-srivastava-03678116b/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/sarvesh.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanuja Pal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joint Finance Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.facebook.com/tanuja.pal.75436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/tanuja.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanya Bhandari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/tanyabhandari25/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/tanya.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anika Sharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketing Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/sharma3anika/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/anika.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajay Chahar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creative Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/ajay-c-200a9b110/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/ajay.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishal Dhiman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joint Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/vishal-dhiman-b99a9b18b/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../members/vishal.jpg</t>
+    <t>https://www.linkedin.com/in/akhyarai/</t>
+  </si>
+  <si>
+    <t>../members/akhya.jpg</t>
+  </si>
+  <si>
+    <t>Abhay Raj Singh Rathod</t>
+  </si>
+  <si>
+    <t>Joint Technical Secretary</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rathod-sahaab/</t>
+  </si>
+  <si>
+    <t>../members/abhay.jpg</t>
+  </si>
+  <si>
+    <t>Aditi Singh</t>
+  </si>
+  <si>
+    <t>PR Head</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aditi-singh2000/</t>
+  </si>
+  <si>
+    <t>../members/aditi.jpg</t>
+  </si>
+  <si>
+    <t>Anshudhar Kumar Singh</t>
+  </si>
+  <si>
+    <t>Technical Secretary</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/anshudhar-kumar-singh/</t>
+  </si>
+  <si>
+    <t>../members/anshudhar.jpg</t>
+  </si>
+  <si>
+    <t>Arsh Sharma</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sov-trotter/</t>
+  </si>
+  <si>
+    <t>../members/arsh.jpg</t>
+  </si>
+  <si>
+    <t>Harshit Srivastav</t>
+  </si>
+  <si>
+    <t>Media Head</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harshit-srivastav-1507/</t>
+  </si>
+  <si>
+    <t>../members/harshit.jpg</t>
+  </si>
+  <si>
+    <t>Nimish Lata</t>
+  </si>
+  <si>
+    <t>Finance Secretary</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nimish-sharma-0b0929195/</t>
+  </si>
+  <si>
+    <t>../members/nimish.jpg</t>
+  </si>
+  <si>
+    <t>Rohan Nawathe</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rnawathe/</t>
+  </si>
+  <si>
+    <t>../members/rohan.jpg</t>
+  </si>
+  <si>
+    <t>Sarvesh Srivastava</t>
+  </si>
+  <si>
+    <t>Vice President</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sarvesh-srivastava-03678116b/</t>
+  </si>
+  <si>
+    <t>../members/sarvesh.jpg</t>
+  </si>
+  <si>
+    <t>Tanuja Pal</t>
+  </si>
+  <si>
+    <t>Joint Finance Secretary</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tanuja.pal.75436</t>
+  </si>
+  <si>
+    <t>../members/tanuja.jpg</t>
+  </si>
+  <si>
+    <t>Tanya Bhandari</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/tanyabhandari25/</t>
+  </si>
+  <si>
+    <t>../members/tanya.jpg</t>
+  </si>
+  <si>
+    <t>Anika Sharma</t>
+  </si>
+  <si>
+    <t>Marketing Head</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sharma3anika/</t>
+  </si>
+  <si>
+    <t>../members/anika.jpg</t>
+  </si>
+  <si>
+    <t>Ajay Chahar</t>
+  </si>
+  <si>
+    <t>Creative Head</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ajay-c-200a9b110/</t>
+  </si>
+  <si>
+    <t>../members/ajay.jpg</t>
+  </si>
+  <si>
+    <t>Vishal Dhiman</t>
+  </si>
+  <si>
+    <t>Joint Secretary</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vishal-dhiman-b99a9b18b/</t>
+  </si>
+  <si>
+    <t>../members/vishal.jpg</t>
+  </si>
+  <si>
+    <t>../members/Harshwardhan.jpeg</t>
+  </si>
+  <si>
+    <t>../members/disha.png</t>
+  </si>
+  <si>
+    <t>Disha Gupta</t>
+  </si>
+  <si>
+    <t>Tanmay Sirvastav</t>
+  </si>
+  <si>
+    <t>../members/tanmay.jpg</t>
+  </si>
+  <si>
+    <t>../members/Meenakshi.jpeg</t>
+  </si>
+  <si>
+    <t>../members/noel.jpg</t>
+  </si>
+  <si>
+    <t>../members/Deepak.jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -580,24 +588,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -609,7 +609,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -617,73 +617,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -742,14 +694,30 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{EB214A6F-56F6-4109-9651-D9E81CFC262A}">
-  <header guid="{7AD1FDD9-3986-4B52-8D24-50E3FA73634A}" dateTime="2021-06-06T15:37:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="1" maxSheetId="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E1360E97-3B9F-4EDC-9492-67F252EB0EAA}" diskRevisions="1" revisionId="9" version="5">
+  <header guid="{BC7F68AF-4C3F-48A4-B048-E81ACA653319}" dateTime="2021-07-22T20:19:00" maxSheetId="5" userName=" " r:id="rId2" minRId="2">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -757,7 +725,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{BC7F68AF-4C3F-48A4-B048-E81ACA653319}" dateTime="2021-07-22T20:19:00.000000000Z" userName=" " r:id="rId2" minRId="2" maxRId="2" maxSheetId="5">
+  <header guid="{51418908-2FF3-4352-97F8-3E8CD4D98DB1}" dateTime="2021-07-22T20:20:00" maxSheetId="5" userName=" " r:id="rId3" minRId="3" maxRId="5">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -765,7 +733,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{51418908-2FF3-4352-97F8-3E8CD4D98DB1}" dateTime="2021-07-22T20:20:00.000000000Z" userName=" " r:id="rId3" minRId="3" maxRId="5" maxSheetId="5">
+  <header guid="{FD922C10-8AAC-4698-8A68-285CCBF06619}" dateTime="2021-07-22T20:21:00" maxSheetId="5" userName=" " r:id="rId4" minRId="6" maxRId="9">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -773,7 +741,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{FD922C10-8AAC-4698-8A68-285CCBF06619}" dateTime="2021-07-22T20:21:00.000000000Z" userName=" " r:id="rId4" minRId="6" maxRId="9" maxSheetId="5">
+  <header guid="{496AD67D-293E-40D4-AAD7-7CB45AA91A79}" dateTime="2021-07-22T20:22:00" maxSheetId="5" userName=" " r:id="rId5" minRId="10" maxRId="11">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -781,7 +749,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{496AD67D-293E-40D4-AAD7-7CB45AA91A79}" dateTime="2021-07-22T20:22:00.000000000Z" userName=" " r:id="rId5" minRId="10" maxRId="11" maxSheetId="5">
+  <header guid="{0A6D860E-51F7-470A-938B-15BD679BA6CF}" dateTime="2021-07-22T20:23:00" maxSheetId="5" userName=" " r:id="rId6" minRId="12" maxRId="15">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -789,7 +757,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{0A6D860E-51F7-470A-938B-15BD679BA6CF}" dateTime="2021-07-22T20:23:00.000000000Z" userName=" " r:id="rId6" minRId="12" maxRId="15" maxSheetId="5">
+  <header guid="{5E5E9331-E9F9-4682-BFC2-80EAD7EF970D}" dateTime="2021-07-22T20:24:00" maxSheetId="5" userName=" " r:id="rId7" minRId="16" maxRId="18">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -797,7 +765,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{5E5E9331-E9F9-4682-BFC2-80EAD7EF970D}" dateTime="2021-07-22T20:24:00.000000000Z" userName=" " r:id="rId7" minRId="16" maxRId="18" maxSheetId="5">
+  <header guid="{F2EC6514-3C12-43EE-A569-0E215CD44702}" dateTime="2021-07-22T20:29:00" maxSheetId="5" userName=" " r:id="rId8" minRId="19" maxRId="98">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -805,7 +773,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{F2EC6514-3C12-43EE-A569-0E215CD44702}" dateTime="2021-07-22T20:29:00.000000000Z" userName=" " r:id="rId8" minRId="19" maxRId="98" maxSheetId="5">
+  <header guid="{2FCD8317-8C95-4D74-AD13-499ED5AD680A}" dateTime="2021-07-22T20:30:00" maxSheetId="5" userName=" " r:id="rId9" minRId="99" maxRId="178">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -813,7 +781,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{2FCD8317-8C95-4D74-AD13-499ED5AD680A}" dateTime="2021-07-22T20:30:00.000000000Z" userName=" " r:id="rId9" minRId="99" maxRId="178" maxSheetId="5">
+  <header guid="{12E8F146-CE30-46FC-ACC4-EECC9218D049}" dateTime="2021-07-22T20:32:00" maxSheetId="5" userName=" " r:id="rId10" minRId="179" maxRId="186">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -821,7 +789,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{12E8F146-CE30-46FC-ACC4-EECC9218D049}" dateTime="2021-07-22T20:32:00.000000000Z" userName=" " r:id="rId10" minRId="179" maxRId="186" maxSheetId="5">
+  <header guid="{36B80032-01EA-4458-B9EC-A78F69A55CCC}" dateTime="2021-07-22T20:33:00" maxSheetId="5" userName=" " r:id="rId11" minRId="187" maxRId="193">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -829,7 +797,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{36B80032-01EA-4458-B9EC-A78F69A55CCC}" dateTime="2021-07-22T20:33:00.000000000Z" userName=" " r:id="rId11" minRId="187" maxRId="193" maxSheetId="5">
+  <header guid="{A7665D57-4B5A-4D08-894E-9FC45DF0C37C}" dateTime="2021-07-22T20:37:00" maxSheetId="5" userName=" " r:id="rId12" minRId="194" maxRId="273">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -837,7 +805,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{A7665D57-4B5A-4D08-894E-9FC45DF0C37C}" dateTime="2021-07-22T20:37:00.000000000Z" userName=" " r:id="rId12" minRId="194" maxRId="273" maxSheetId="5">
+  <header guid="{12529915-C486-4ADB-9924-D29528F51226}" dateTime="2021-07-22T20:41:00" maxSheetId="5" userName=" " r:id="rId13" minRId="274" maxRId="358">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -845,7 +813,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{12529915-C486-4ADB-9924-D29528F51226}" dateTime="2021-07-22T20:41:00.000000000Z" userName=" " r:id="rId13" minRId="274" maxRId="358" maxSheetId="5">
+  <header guid="{13C03921-40F7-4450-A94D-2FB3FDB41BBF}" dateTime="2021-07-22T20:42:00" maxSheetId="5" userName=" " r:id="rId14" minRId="359" maxRId="370">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -853,7 +821,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{13C03921-40F7-4450-A94D-2FB3FDB41BBF}" dateTime="2021-07-22T20:42:00.000000000Z" userName=" " r:id="rId14" minRId="359" maxRId="370" maxSheetId="5">
+  <header guid="{B71AE3A7-223E-46A5-B502-1A719664D743}" dateTime="2021-07-22T20:43:00" maxSheetId="5" userName=" " r:id="rId15" minRId="371" maxRId="374">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -861,7 +829,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{B71AE3A7-223E-46A5-B502-1A719664D743}" dateTime="2021-07-22T20:43:00.000000000Z" userName=" " r:id="rId15" minRId="371" maxRId="374" maxSheetId="5">
+  <header guid="{9CE4A2C8-98EB-4882-9864-E793A1DDB822}" dateTime="2021-07-22T20:45:00" maxSheetId="5" userName=" " r:id="rId16" minRId="375" maxRId="377">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -869,7 +837,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{9CE4A2C8-98EB-4882-9864-E793A1DDB822}" dateTime="2021-07-22T20:45:00.000000000Z" userName=" " r:id="rId16" minRId="375" maxRId="377" maxSheetId="5">
+  <header guid="{B21AD75E-ED21-4E4C-A017-1E4AA5A9B931}" dateTime="2021-07-22T20:46:00" maxSheetId="5" userName=" " r:id="rId17" minRId="378" maxRId="389">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -877,7 +845,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{B21AD75E-ED21-4E4C-A017-1E4AA5A9B931}" dateTime="2021-07-22T20:46:00.000000000Z" userName=" " r:id="rId17" minRId="378" maxRId="389" maxSheetId="5">
+  <header guid="{8CA25868-6DB8-468A-B4B7-5DED89D12955}" dateTime="2021-07-22T20:47:00" maxSheetId="5" userName=" " r:id="rId18" minRId="390" maxRId="475">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -885,7 +853,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{8CA25868-6DB8-468A-B4B7-5DED89D12955}" dateTime="2021-07-22T20:47:00.000000000Z" userName=" " r:id="rId18" minRId="390" maxRId="475" maxSheetId="5">
+  <header guid="{CE5A2FF5-616E-435E-AE17-3BB0F6EEF019}" dateTime="2021-07-22T20:48:00" maxSheetId="5" userName=" " r:id="rId19" minRId="476" maxRId="575">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -893,7 +861,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{CE5A2FF5-616E-435E-AE17-3BB0F6EEF019}" dateTime="2021-07-22T20:48:00.000000000Z" userName=" " r:id="rId19" minRId="476" maxRId="575" maxSheetId="5">
+  <header guid="{87E2B619-D1A5-4EE7-AB2E-F6B0FD0C1359}" dateTime="2021-07-22T21:00:00" maxSheetId="5" userName=" " r:id="rId20" minRId="576" maxRId="577">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -901,7 +869,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{87E2B619-D1A5-4EE7-AB2E-F6B0FD0C1359}" dateTime="2021-07-22T21:00:00.000000000Z" userName=" " r:id="rId20" minRId="576" maxRId="577" maxSheetId="5">
+  <header guid="{9D57F045-860C-4827-B905-0CC6357A3EAB}" dateTime="2021-07-22T21:01:00" maxSheetId="5" userName=" " r:id="rId21" minRId="578" maxRId="594">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -909,7 +877,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{9D57F045-860C-4827-B905-0CC6357A3EAB}" dateTime="2021-07-22T21:01:00.000000000Z" userName=" " r:id="rId21" minRId="578" maxRId="594" maxSheetId="5">
+  <header guid="{65C6672D-2260-476A-A78B-1D1617F546A2}" dateTime="2021-07-22T21:02:00" maxSheetId="5" userName=" " r:id="rId22" minRId="595" maxRId="607">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -917,7 +885,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{65C6672D-2260-476A-A78B-1D1617F546A2}" dateTime="2021-07-22T21:02:00.000000000Z" userName=" " r:id="rId22" minRId="595" maxRId="607" maxSheetId="5">
+  <header guid="{DF55E8A2-AA68-4910-AE6A-C8BA6BECF6CA}" dateTime="2021-07-22T21:03:00" maxSheetId="5" userName=" " r:id="rId23" minRId="608" maxRId="613">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -925,7 +893,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{DF55E8A2-AA68-4910-AE6A-C8BA6BECF6CA}" dateTime="2021-07-22T21:03:00.000000000Z" userName=" " r:id="rId23" minRId="608" maxRId="613" maxSheetId="5">
+  <header guid="{6AC4F327-C9EB-4B9F-8840-DCC480269B40}" dateTime="2021-07-22T21:13:00" maxSheetId="5" userName=" " r:id="rId24" minRId="614">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -933,7 +901,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{6AC4F327-C9EB-4B9F-8840-DCC480269B40}" dateTime="2021-07-22T21:13:00.000000000Z" userName=" " r:id="rId24" minRId="614" maxRId="614" maxSheetId="5">
+  <header guid="{E16B699B-9FB2-4BE0-81B1-14741BC5D804}" dateTime="2021-07-22T21:15:00" maxSheetId="5" userName=" " r:id="rId25" minRId="615">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -941,7 +909,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{E16B699B-9FB2-4BE0-81B1-14741BC5D804}" dateTime="2021-07-22T21:15:00.000000000Z" userName=" " r:id="rId25" minRId="615" maxRId="615" maxSheetId="5">
+  <header guid="{0A1465B8-9605-4F21-8F33-19D1ED84D6D9}" dateTime="2021-07-22T21:18:00" maxSheetId="5" userName=" " r:id="rId26" minRId="616">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -949,7 +917,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{0A1465B8-9605-4F21-8F33-19D1ED84D6D9}" dateTime="2021-07-22T21:18:00.000000000Z" userName=" " r:id="rId26" minRId="616" maxRId="616" maxSheetId="5">
+  <header guid="{7FBA8CA5-B4BA-46B5-952E-0C5EA525424C}" dateTime="2021-07-22T21:19:00" maxSheetId="5" userName=" " r:id="rId27" minRId="617">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -957,7 +925,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{7FBA8CA5-B4BA-46B5-952E-0C5EA525424C}" dateTime="2021-07-22T21:19:00.000000000Z" userName=" " r:id="rId27" minRId="617" maxRId="617" maxSheetId="5">
+  <header guid="{BCD2DDD7-0B73-4E2C-83AF-5DB0FA66510F}" dateTime="2021-07-22T21:20:00" maxSheetId="5" userName=" " r:id="rId28" minRId="618" maxRId="619">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -965,7 +933,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{BCD2DDD7-0B73-4E2C-83AF-5DB0FA66510F}" dateTime="2021-07-22T21:20:00.000000000Z" userName=" " r:id="rId28" minRId="618" maxRId="619" maxSheetId="5">
+  <header guid="{65450A33-AAD8-42E6-8CD5-3FC810546D3E}" dateTime="2021-07-22T21:21:00" maxSheetId="5" userName=" " r:id="rId29" minRId="620">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -973,7 +941,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{65450A33-AAD8-42E6-8CD5-3FC810546D3E}" dateTime="2021-07-22T21:21:00.000000000Z" userName=" " r:id="rId29" minRId="620" maxRId="620" maxSheetId="5">
+  <header guid="{C7BC7030-DFA0-4459-8E3D-11693136C459}" dateTime="2021-07-22T21:22:00" maxSheetId="5" userName=" " r:id="rId30" minRId="621">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -981,7 +949,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{C7BC7030-DFA0-4459-8E3D-11693136C459}" dateTime="2021-07-22T21:22:00.000000000Z" userName=" " r:id="rId30" minRId="621" maxRId="621" maxSheetId="5">
+  <header guid="{290C2F2C-7ED8-4F55-8838-2932614A2038}" dateTime="2021-07-22T21:24:00" maxSheetId="5" userName=" " r:id="rId31" minRId="622">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -989,7 +957,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{290C2F2C-7ED8-4F55-8838-2932614A2038}" dateTime="2021-07-22T21:24:00.000000000Z" userName=" " r:id="rId31" minRId="622" maxRId="622" maxSheetId="5">
+  <header guid="{89B23809-0032-4472-B4EA-936863FAA67B}" dateTime="2021-07-22T21:26:00" maxSheetId="5" userName=" " r:id="rId32" minRId="623">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -997,7 +965,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{89B23809-0032-4472-B4EA-936863FAA67B}" dateTime="2021-07-22T21:26:00.000000000Z" userName=" " r:id="rId32" minRId="623" maxRId="623" maxSheetId="5">
+  <header guid="{36CF003C-B488-4A88-A154-2874D766B4BB}" dateTime="2021-07-22T21:33:00" maxSheetId="5" userName=" " r:id="rId33" minRId="624">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1005,7 +973,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{36CF003C-B488-4A88-A154-2874D766B4BB}" dateTime="2021-07-22T21:33:00.000000000Z" userName=" " r:id="rId33" minRId="624" maxRId="624" maxSheetId="5">
+  <header guid="{EB214A6F-56F6-4109-9651-D9E81CFC262A}" dateTime="2021-07-22T21:35:00" maxSheetId="5" userName=" " r:id="rId34" minRId="625">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1013,7 +981,31 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{EB214A6F-56F6-4109-9651-D9E81CFC262A}" dateTime="2021-07-22T21:35:00.000000000Z" userName=" " r:id="rId34" minRId="625" maxRId="625" maxSheetId="5">
+  <header guid="{81C46309-F68E-4FBF-B7F7-3BF0FF122B9D}" dateTime="2021-08-17T20:03:41" maxSheetId="5" userName="Sumit Dhiman" r:id="rId35" minRId="1" maxRId="6">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6197EE08-DFE4-4B9D-AAAF-7AD146A633CF}" dateTime="2021-08-17T20:04:13" maxSheetId="5" userName="Sumit Dhiman" r:id="rId36" minRId="7">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DD991DC5-FF18-4F75-8F28-4443A22215E5}" dateTime="2021-08-17T20:04:43" maxSheetId="5" userName="Sumit Dhiman" r:id="rId37" minRId="8">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E1360E97-3B9F-4EDC-9492-67F252EB0EAA}" dateTime="2021-08-17T20:07:54" maxSheetId="5" userName="Sumit Dhiman" r:id="rId38" minRId="9">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1024,39 +1016,6 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="1" ua="false" sId="3">
-    <oc r="A3" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Aakhya Rai</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="A3" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Akhya Rai</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="179" ua="false" sId="4">
@@ -9987,6 +9946,135 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="2">
+    <oc r="E8" t="inlineStr">
+      <is>
+        <t>../members/Harshwardhan.jpg</t>
+      </is>
+    </oc>
+    <nc r="E8" t="inlineStr">
+      <is>
+        <t>../members/Harshwardhan.jpeg</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" sId="2">
+    <oc r="E11" t="inlineStr">
+      <is>
+        <t>../members/Lovekesh.jpeg</t>
+      </is>
+    </oc>
+    <nc r="E11" t="inlineStr">
+      <is>
+        <t>../members/disha.png</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="3" sId="2">
+    <oc r="D11" t="inlineStr">
+      <is>
+        <t>https://www.linkedin.com/in/lovekesh-bansal-123786191</t>
+      </is>
+    </oc>
+    <nc r="D11" t="inlineStr">
+      <is>
+        <t>https://www.istenith.com/</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="4" sId="2">
+    <oc r="A11" t="inlineStr">
+      <is>
+        <t>Lovkesh Bansal</t>
+      </is>
+    </oc>
+    <nc r="A11" t="inlineStr">
+      <is>
+        <t>Disha Gupta</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="5" sId="2">
+    <oc r="A12" t="inlineStr">
+      <is>
+        <t>Mayank Thakur</t>
+      </is>
+    </oc>
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>Tanmay Sirvastav</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" sId="2">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>../members/Mayank2.jpg</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>../members/tanmay.jpg</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{DF53FF45-CD95-46C9-A254-8606AC4BE6BE}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="7" sId="2">
+    <oc r="E13" t="inlineStr">
+      <is>
+        <t>../members/Meenakshi.jpg</t>
+      </is>
+    </oc>
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>../members/Meenakshi.jpeg</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="8" sId="2">
+    <oc r="E14" t="inlineStr">
+      <is>
+        <t>../members/noel.jpeg</t>
+      </is>
+    </oc>
+    <nc r="E14" t="inlineStr">
+      <is>
+        <t>../members/noel.jpg</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="9" sId="2">
+    <oc r="E3" t="inlineStr">
+      <is>
+        <t>../members/Deepak.jpg</t>
+      </is>
+    </oc>
+    <nc r="E3" t="inlineStr">
+      <is>
+        <t>../members/Deepak.jpeg</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="6" ua="false" sId="3">
@@ -13051,28 +13139,318 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.22"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13089,7 +13467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -13106,7 +13484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -13123,7 +13501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -13140,7 +13518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -13157,7 +13535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -13174,7 +13552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -13191,7 +13569,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -13208,7 +13586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -13225,7 +13603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -13242,7 +13620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -13259,7 +13637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -13276,7 +13654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -13293,7 +13671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -13310,7 +13688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -13327,7 +13705,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -13344,7 +13722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -13361,7 +13739,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -13378,7 +13756,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -13395,7 +13773,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -13412,61 +13790,56 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DF53FF45-CD95-46C9-A254-8606AC4BE6BE}">
+      <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+      <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+  </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.istenith.com/"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.istenith.com/"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://www.istenith.com/"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://www.istenith.com/"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://www.istenith.com/"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://www.istenith.com/"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://www.istenith.com/"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://www.istenith.com/"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://www.istenith.com/"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://www.istenith.com/"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://www.istenith.com/"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://www.istenith.com/"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://www.istenith.com/"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://www.istenith.com/"/>
-    <hyperlink ref="D16" r:id="rId15" display="https://www.istenith.com/"/>
-    <hyperlink ref="D17" r:id="rId16" display="https://www.istenith.com/"/>
-    <hyperlink ref="D18" r:id="rId17" display="https://www.istenith.com/"/>
-    <hyperlink ref="D19" r:id="rId18" display="https://www.istenith.com/"/>
-    <hyperlink ref="D20" r:id="rId19" display="https://www.istenith.com/"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.78"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13483,7 +13856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -13500,7 +13873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -13514,10 +13887,10 @@
         <v>49</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -13534,7 +13907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -13551,7 +13924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -13568,7 +13941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -13585,7 +13958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -13599,10 +13972,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -13619,7 +13992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -13636,9 +14009,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>169</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>46</v>
@@ -13647,15 +14020,15 @@
         <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>170</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>46</v>
@@ -13667,10 +14040,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>171</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -13681,13 +14054,13 @@
         <v>47</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -13698,13 +14071,13 @@
         <v>47</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -13721,7 +14094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -13732,13 +14105,13 @@
         <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -13755,7 +14128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -13766,13 +14139,13 @@
         <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -13783,13 +14156,13 @@
         <v>47</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -13807,31 +14180,41 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DF53FF45-CD95-46C9-A254-8606AC4BE6BE}">
+      <selection activeCell="E12" sqref="E12"/>
+      <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+      <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+      <headerFooter>
+        <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+        <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.linkedin.com/in/albert-sharma-2016"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.linkedin.com/in/deepak-singh-a04ba51ba/"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://www.linkedin.com/in/dev-khanduja/"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://www.linkedin.com/in/divyansh-tripathi-4bb66a205"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://www.istenith.com/"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://www.istenith.com/"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://www.istenith.com/"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://www.linkedin.com/in/kartik-576b24205"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://www.linkedin.com/in/vermakaustubh28/"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://www.linkedin.com/in/lovekesh-bansal-123786191"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://www.istenith.com/"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://www.linkedin.com/in/meenakshi-33b683205"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://www.linkedin.com/in/noel-kankipati-444b1a217/"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://www.istenith.com/"/>
-    <hyperlink ref="D16" r:id="rId15" display="https://www.linkedin.com/in/shriya-chauhan-20a19b200"/>
-    <hyperlink ref="D17" r:id="rId16" display="https://www.istenith.com/"/>
-    <hyperlink ref="D18" r:id="rId17" display="https://www.linkedin.com/in/sumit-dhiman-20bce091"/>
-    <hyperlink ref="D19" r:id="rId18" display="https://www.linkedin.com/in/vansh-thakur-b029a4202/"/>
-    <hyperlink ref="D20" r:id="rId19" display="https://www.istenith.com/"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" display="https://www.linkedin.com/in/lovekesh-bansal-123786191" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -13839,25 +14222,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.03"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13874,292 +14254,302 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>67</v>
+      <c r="D4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>70</v>
+      <c r="D5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>73</v>
+      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>76</v>
+      <c r="D7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>79</v>
+      <c r="D8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>82</v>
+      <c r="D9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>90</v>
+      <c r="D12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>93</v>
+      <c r="D13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>96</v>
+      <c r="D14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>99</v>
+      <c r="D15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>102</v>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="D17" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" t="s">
         <v>107</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DF53FF45-CD95-46C9-A254-8606AC4BE6BE}">
+      <selection activeCell="D6" sqref="D6"/>
+      <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+      <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+      <headerFooter>
+        <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+        <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.linkedin.com/in/gaurav-pandey-412180194/"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.linkedin.com/in/kunal-thakur-b27823193/"/>
-    <hyperlink ref="D7" r:id="rId3" display="https://www.linkedin.com/in/mayur-kumar-47a9511a1/"/>
-    <hyperlink ref="D8" r:id="rId4" display="https://www.linkedin.com/in/parasaggarwal/"/>
-    <hyperlink ref="D9" r:id="rId5" display="https://www.linkedin.com/in/parth-pant-866bb4189/"/>
-    <hyperlink ref="D10" r:id="rId6" display="https://www.istenith.com/"/>
-    <hyperlink ref="D13" r:id="rId7" display="https://www.linkedin.com/in/uditee-singh-7619921b0/"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -14167,26 +14557,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.14"/>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14203,281 +14590,291 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="5" t="s">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>121</v>
+      <c r="D10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>125</v>
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>129</v>
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>133</v>
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>137</v>
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>141</v>
+    <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>162</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>144</v>
+    <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>166</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DF53FF45-CD95-46C9-A254-8606AC4BE6BE}">
+      <selection activeCell="C19" sqref="C19"/>
+      <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+      <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+      <headerFooter>
+        <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+        <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="https://www.linkedin.com/in/rathod-sahaab/"/>
-    <hyperlink ref="D5" r:id="rId2" display="https://www.linkedin.com/in/aditi-singh2000/"/>
-    <hyperlink ref="D7" r:id="rId3" display="https://www.linkedin.com/in/sov-trotter/"/>
-    <hyperlink ref="D8" r:id="rId4" display="https://www.linkedin.com/in/harshit-srivastav-1507/"/>
-    <hyperlink ref="D10" r:id="rId5" display="https://www.linkedin.com/in/rnawathe/"/>
-    <hyperlink ref="D11" r:id="rId6" display="https://www.linkedin.com/in/sarvesh-srivastava-03678116b/"/>
-    <hyperlink ref="D14" r:id="rId7" display="https://www.linkedin.com/in/sharma3anika/"/>
-    <hyperlink ref="D16" r:id="rId8" display="https://www.linkedin.com/in/vishal-dhiman-b99a9b18b/"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="D14" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="D16" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
updated member's image and desc
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="365">
   <si>
     <t>name</t>
   </si>
@@ -669,7 +669,7 @@
     <t>../members/gaurav2.webp</t>
   </si>
   <si>
-    <t xml:space="preserve">Batch 2023</t>
+    <t xml:space="preserve">Effective Engineering Student committed to learning, developing skills and team contribution. Self-directed and energetic. My fields of interest are software development and Artificial Intelligence/Machine Learning.</t>
   </si>
   <si>
     <t xml:space="preserve">Gaurav Pandey</t>
@@ -733,6 +733,9 @@
   </si>
   <si>
     <t>Udaipur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Mayur Kumar</t>
@@ -29086,7 +29089,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -29346,31 +29349,31 @@
         <v>121</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K7" s="17"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>82</v>
@@ -29379,13 +29382,13 @@
         <v>83</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K8" s="17"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>208</v>
@@ -29394,10 +29397,10 @@
         <v>214</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>53</v>
@@ -29406,31 +29409,31 @@
         <v>138</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>18</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K9" s="17"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>60</v>
@@ -29445,25 +29448,25 @@
         <v>37</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K10" s="17"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>102</v>
@@ -29478,25 +29481,25 @@
         <v>18</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K11" s="17"/>
     </row>
     <row r="12" ht="17.25" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>147</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>65</v>
@@ -29509,25 +29512,25 @@
         <v>37</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K12" s="17"/>
     </row>
     <row r="13" ht="17.25" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>71</v>
@@ -29536,31 +29539,31 @@
         <v>143</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K13" s="17"/>
     </row>
     <row r="14" ht="17.25" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>80</v>
@@ -29569,31 +29572,31 @@
         <v>54</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>37</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K14" s="17"/>
     </row>
     <row r="15" ht="17.25" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>75</v>
@@ -29608,31 +29611,31 @@
         <v>37</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K15" s="17"/>
     </row>
     <row r="16" ht="17.25" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>86</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>193</v>
@@ -29641,31 +29644,31 @@
         <v>18</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K16" s="17"/>
     </row>
     <row r="17" ht="17.25" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>24</v>
@@ -29674,7 +29677,7 @@
         <v>18</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="K17" s="17"/>
     </row>
@@ -42600,52 +42603,52 @@
     </row>
     <row r="2" ht="17.25" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K2" s="32"/>
     </row>
     <row r="3" ht="17.25" customHeight="1">
       <c r="A3" s="30" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>34</v>
@@ -42654,31 +42657,31 @@
         <v>132</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K3" s="32"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="30" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>90</v>
@@ -42693,25 +42696,25 @@
         <v>37</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="30" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>23</v>
@@ -42720,31 +42723,31 @@
         <v>103</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>37</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
       <c r="A6" s="30" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>86</v>
@@ -42759,25 +42762,25 @@
         <v>18</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K6" s="32"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
       <c r="A7" s="30" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>41</v>
@@ -42786,64 +42789,64 @@
         <v>132</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="K7" s="32"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
       <c r="A8" s="30" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K8" s="32"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="30" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>53</v>
@@ -42858,25 +42861,25 @@
         <v>37</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K9" s="32"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="30" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>60</v>
@@ -42891,58 +42894,58 @@
         <v>121</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K10" s="32"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
       <c r="A11" s="30" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>65</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K11" s="32"/>
     </row>
     <row r="12" ht="17.25" customHeight="1">
       <c r="A12" s="30" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>71</v>
@@ -42951,31 +42954,31 @@
         <v>132</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>37</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K12" s="32"/>
     </row>
     <row r="13" ht="17.25" customHeight="1">
       <c r="A13" s="30" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>75</v>
@@ -42984,31 +42987,31 @@
         <v>35</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>37</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K13" s="32"/>
     </row>
     <row r="14" ht="17.25" customHeight="1">
       <c r="A14" s="30" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F14" s="27" t="s">
         <v>80</v>
@@ -43017,31 +43020,31 @@
         <v>132</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K14" s="32"/>
     </row>
     <row r="15" ht="17.25" customHeight="1">
       <c r="A15" s="30" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>97</v>
@@ -43056,40 +43059,40 @@
         <v>18</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="K15" s="32"/>
     </row>
     <row r="16" ht="17.25" customHeight="1">
       <c r="A16" s="30" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="K16" s="32"/>
     </row>

</xml_diff>

<commit_message>
updated member's year status
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">Abhay Sood</t>
   </si>
   <si>
-    <t>Second</t>
+    <t>first</t>
   </si>
   <si>
     <t xml:space="preserve">Executive Member</t>
@@ -1903,7 +1903,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new members added-2nd yr
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,9 +415,41 @@
         <v>about</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Aditya Rana</v>
+      </c>
+      <c r="B2" t="str">
+        <v>first</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Volunteer Member</v>
+      </c>
+      <c r="D2" t="str">
+        <v>https://www.linkedin.com/in/aditya-rana-6156071aa</v>
+      </c>
+      <c r="E2" t="str">
+        <v>../members/aditiya.webp</v>
+      </c>
+      <c r="F2" t="str">
+        <v>1LjuDNVhaQmaOaujbP3XWpNtAaXtnAZNo</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Computer science and Engineering</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Kangra</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Himachal Pradesh</v>
+      </c>
+      <c r="J2" t="str">
+        <v>I am an instance of my own class | Fresher @ CSE NITH | Always learning and implementing latest and greatest technologies | Freelancer @ fiverr | Android Developer |</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Aditya Rana</v>
+        <v>Armaan Shukla</v>
       </c>
       <c r="B3" t="str">
         <v>first</v>
@@ -425,17 +457,14 @@
       <c r="C3" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D3" t="str">
-        <v>https://www.linkedin.com/in/aditya-rana-6156071aa</v>
-      </c>
       <c r="E3" t="str">
-        <v>../members/aditiya.webp</v>
+        <v>../members/armaan.webp</v>
       </c>
       <c r="F3" t="str">
-        <v>1LjuDNVhaQmaOaujbP3XWpNtAaXtnAZNo</v>
+        <v>1Tpnk2k0ZIv73FWy7JeLxcRBjC_Oq7O-f</v>
       </c>
       <c r="G3" t="str">
-        <v>Computer science and Engineering</v>
+        <v>Mathematics and Computing</v>
       </c>
       <c r="H3" t="str">
         <v>Kangra</v>
@@ -444,12 +473,12 @@
         <v>Himachal Pradesh</v>
       </c>
       <c r="J3" t="str">
-        <v>I am an instance of my own class | Fresher @ CSE NITH | Always learning and implementing latest and greatest technologies | Freelancer @ fiverr | Android Developer |</v>
+        <v>Batch 2025</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Armaan Shukla</v>
+        <v>Chandan Kumar</v>
       </c>
       <c r="B4" t="str">
         <v>first</v>
@@ -457,20 +486,23 @@
       <c r="C4" t="str">
         <v>Volunteer Member</v>
       </c>
+      <c r="D4" t="str">
+        <v>https://www.linkedin.com/in/chandan-kumar-19880a22a/</v>
+      </c>
       <c r="E4" t="str">
-        <v>../members/armaan.webp</v>
+        <v>../members/chandan.webp</v>
       </c>
       <c r="F4" t="str">
-        <v>1Tpnk2k0ZIv73FWy7JeLxcRBjC_Oq7O-f</v>
+        <v>1522oz7z6THBgb0FxF4DmHlyI3YQpviNM</v>
       </c>
       <c r="G4" t="str">
-        <v>Mathematics and Computing</v>
+        <v>Electronics and Communication Engineering</v>
       </c>
       <c r="H4" t="str">
-        <v>Kangra</v>
+        <v>Varanasi</v>
       </c>
       <c r="I4" t="str">
-        <v>Himachal Pradesh</v>
+        <v>Uttar Pradesh</v>
       </c>
       <c r="J4" t="str">
         <v>Batch 2025</v>
@@ -478,7 +510,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Chandan Kumar</v>
+        <v>Charu</v>
       </c>
       <c r="B5" t="str">
         <v>first</v>
@@ -487,22 +519,22 @@
         <v>Volunteer Member</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.linkedin.com/in/chandan-kumar-19880a22a/</v>
+        <v>https://www.linkedin.com/in/charu-229665223</v>
       </c>
       <c r="E5" t="str">
-        <v>../members/chandan.webp</v>
+        <v>../members/charu.webp</v>
       </c>
       <c r="F5" t="str">
-        <v>1522oz7z6THBgb0FxF4DmHlyI3YQpviNM</v>
+        <v>1gYhb-XoUU6OsD2Zrk-eqEUR94UtYotqJ</v>
       </c>
       <c r="G5" t="str">
-        <v>Electronics and Communication Engineering</v>
+        <v xml:space="preserve">Mechanical Engineering </v>
       </c>
       <c r="H5" t="str">
-        <v>Varanasi</v>
+        <v>Kangra</v>
       </c>
       <c r="I5" t="str">
-        <v>Uttar Pradesh</v>
+        <v xml:space="preserve">Himachal Pradesh </v>
       </c>
       <c r="J5" t="str">
         <v>Batch 2025</v>
@@ -510,7 +542,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Charu</v>
+        <v xml:space="preserve">Dharuva Thakur </v>
       </c>
       <c r="B6" t="str">
         <v>first</v>
@@ -519,19 +551,19 @@
         <v>Volunteer Member</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.linkedin.com/in/charu-229665223</v>
+        <v>https://www.linkedin.com/in/dharuva-thakur-83576122a</v>
       </c>
       <c r="E6" t="str">
-        <v>../members/charu.webp</v>
+        <v>../members/dharuva.webp</v>
       </c>
       <c r="F6" t="str">
-        <v>1gYhb-XoUU6OsD2Zrk-eqEUR94UtYotqJ</v>
+        <v>18hlg1lzF81JB-DJKg36G5SHzOM2zB7Xz</v>
       </c>
       <c r="G6" t="str">
-        <v xml:space="preserve">Mechanical Engineering </v>
+        <v>Mathematics and Scientific Computing</v>
       </c>
       <c r="H6" t="str">
-        <v>Kangra</v>
+        <v>Mandi</v>
       </c>
       <c r="I6" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
@@ -542,7 +574,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v xml:space="preserve">Dharuva Thakur </v>
+        <v>Ekansh Verma</v>
       </c>
       <c r="B7" t="str">
         <v>first</v>
@@ -551,30 +583,30 @@
         <v>Volunteer Member</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.linkedin.com/in/dharuva-thakur-83576122a</v>
+        <v>https://www.linkedin.com/in/ekansh-verma-469557228</v>
       </c>
       <c r="E7" t="str">
-        <v>../members/dharuva.webp</v>
+        <v>../members/ekansh.webp</v>
       </c>
       <c r="F7" t="str">
-        <v>18hlg1lzF81JB-DJKg36G5SHzOM2zB7Xz</v>
+        <v>1upS_dc_SLM0CsaA__dVnXqApgS4eFKD1</v>
       </c>
       <c r="G7" t="str">
-        <v>Mathematics and Scientific Computing</v>
+        <v>Electrical Engineering</v>
       </c>
       <c r="H7" t="str">
-        <v>Mandi</v>
+        <v>Kullu</v>
       </c>
       <c r="I7" t="str">
-        <v xml:space="preserve">Himachal Pradesh </v>
+        <v>Himachal Pradesh</v>
       </c>
       <c r="J7" t="str">
-        <v>Batch 2025</v>
+        <v>First Year UG at NiTH</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Ekansh Verma</v>
+        <v>Gargi Dhawan</v>
       </c>
       <c r="B8" t="str">
         <v>first</v>
@@ -583,30 +615,30 @@
         <v>Volunteer Member</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.linkedin.com/in/ekansh-verma-469557228</v>
+        <v>https://www.linkedin.com/in/gargi-dhawan-7706a722a</v>
       </c>
       <c r="E8" t="str">
-        <v>../members/ekansh.webp</v>
+        <v>../members/gargi.webp</v>
       </c>
       <c r="F8" t="str">
-        <v>1upS_dc_SLM0CsaA__dVnXqApgS4eFKD1</v>
+        <v>1HD-obHJOhcS0BYxzv4SRHdRGRnCJ4d-H</v>
       </c>
       <c r="G8" t="str">
-        <v>Electrical Engineering</v>
+        <v>Electronics and Communication Engineering</v>
       </c>
       <c r="H8" t="str">
-        <v>Kullu</v>
+        <v>Shimla</v>
       </c>
       <c r="I8" t="str">
-        <v>Himachal Pradesh</v>
+        <v>Himacha pradesh</v>
       </c>
       <c r="J8" t="str">
-        <v>First Year UG at NiTH</v>
+        <v>Batch 2025</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Gargi Dhawan</v>
+        <v>Hardik Sachdeva</v>
       </c>
       <c r="B9" t="str">
         <v>first</v>
@@ -615,25 +647,25 @@
         <v>Volunteer Member</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.linkedin.com/in/gargi-dhawan-7706a722a</v>
+        <v>https://www.linkedin.com/in/hardik-sachdeva-a69987217</v>
       </c>
       <c r="E9" t="str">
-        <v>../members/gargi.webp</v>
+        <v>../members/hardik.webp</v>
       </c>
       <c r="F9" t="str">
-        <v>1HD-obHJOhcS0BYxzv4SRHdRGRnCJ4d-H</v>
+        <v/>
       </c>
       <c r="G9" t="str">
-        <v>Electronics and Communication Engineering</v>
+        <v>Mathematics and Scientific Computing</v>
       </c>
       <c r="H9" t="str">
-        <v>Shimla</v>
+        <v>Nainital</v>
       </c>
       <c r="I9" t="str">
-        <v>Himacha pradesh</v>
+        <v>Uttarakhand</v>
       </c>
       <c r="J9" t="str">
-        <v>Batch 2025</v>
+        <v>Pursuing BTech in Mathematics And Computing (2025), Interested in Tech. And Financial Stuff. Travel Freak</v>
       </c>
     </row>
     <row r="10">
@@ -856,71 +888,62 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Shariq Verma</v>
+        <v>Shashank Shekhar</v>
       </c>
       <c r="B17" t="str">
         <v>first</v>
       </c>
       <c r="C17" t="str">
-        <v>Volunteer  Member</v>
-      </c>
-      <c r="D17" t="str">
-        <v>https://www.linkedin.com/in/shariq-verma-94a75122a</v>
+        <v>Volenteer Member</v>
       </c>
       <c r="E17" t="str">
-        <v>../members/Shariq.webp</v>
-      </c>
-      <c r="F17" t="str">
-        <v>1KC9wcQ5DgKU31KofULgTIa5VIsbtrttt</v>
-      </c>
-      <c r="G17" t="str">
-        <v>Civil Engineering</v>
+        <v>../members/shashank.webp</v>
       </c>
       <c r="H17" t="str">
-        <v>Shimla</v>
+        <v>Jamui</v>
       </c>
       <c r="I17" t="str">
-        <v>Himachal Pradesh</v>
+        <v>Bihar</v>
       </c>
       <c r="J17" t="str">
-        <v xml:space="preserve">A Civil Engineering Undergraduate interested in core and currently working on core based technical skills. </v>
+        <v>Batch 2025</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Siya Rana</v>
+        <v>Shariq Verma</v>
       </c>
       <c r="B18" t="str">
         <v>first</v>
       </c>
       <c r="C18" t="str">
-        <v>Volunteer Member</v>
+        <v>Volunteer  Member</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.linkedin.com/in/siya-rana-b07639221</v>
+        <v>https://www.linkedin.com/in/shariq-verma-94a75122a</v>
       </c>
       <c r="E18" t="str">
-        <v>../members/siya.webp</v>
+        <v>../members/Shariq.webp</v>
       </c>
       <c r="F18" t="str">
-        <v>1K4LpZE6yPe1EAsxK6zL7RwGDRhvTk97t</v>
+        <v>1KC9wcQ5DgKU31KofULgTIa5VIsbtrttt</v>
       </c>
       <c r="G18" t="str">
-        <v>Electronics and Communication Engineering</v>
+        <v>Civil Engineering</v>
       </c>
       <c r="H18" t="str">
-        <v>Kangra</v>
+        <v>Shimla</v>
       </c>
       <c r="I18" t="str">
         <v>Himachal Pradesh</v>
       </c>
       <c r="J18" t="str">
-        <v>First year student at Nit Hamirpur, pursuing Electronics and Communication Engineering.</v>
+        <v xml:space="preserve">A Civil Engineering Undergraduate interested in core and currently working on core based technical skills. </v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Swastik Sharma</v>
+        <v>Siya Rana</v>
       </c>
       <c r="B19" t="str">
         <v>first</v>
@@ -929,30 +952,62 @@
         <v>Volunteer Member</v>
       </c>
       <c r="D19" t="str">
+        <v>https://www.linkedin.com/in/siya-rana-b07639221</v>
+      </c>
+      <c r="E19" t="str">
+        <v>../members/siya.webp</v>
+      </c>
+      <c r="F19" t="str">
+        <v>1K4LpZE6yPe1EAsxK6zL7RwGDRhvTk97t</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Electronics and Communication Engineering</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Kangra</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Himachal Pradesh</v>
+      </c>
+      <c r="J19" t="str">
+        <v>First year student at Nit Hamirpur, pursuing Electronics and Communication Engineering.</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Swastik Sharma</v>
+      </c>
+      <c r="B20" t="str">
+        <v>first</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Volunteer Member</v>
+      </c>
+      <c r="D20" t="str">
         <v>https://www.linkedin.com/in/swastkk</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E20" t="str">
         <v>../members/Swastik.webp</v>
       </c>
-      <c r="F19" t="str">
+      <c r="F20" t="str">
         <v>15p06FU4eSbaUxpU2A1mq4bD9BS5PxPxu</v>
       </c>
-      <c r="G19" t="str">
+      <c r="G20" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H19" t="str">
+      <c r="H20" t="str">
         <v>UNA</v>
       </c>
-      <c r="I19" t="str">
-        <v>Himachal Pradesh</v>
-      </c>
-      <c r="J19" t="str">
+      <c r="I20" t="str">
+        <v>Himachal Pradesh</v>
+      </c>
+      <c r="J20" t="str">
         <v>A CE Undergrad at NIT Hamirpur currently learning new Web Technologies at Top pace.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J20"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
made 2nd yr -executiveMembers
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -423,7 +423,7 @@
         <v>first</v>
       </c>
       <c r="C2" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D2" t="str">
         <v>https://www.linkedin.com/in/aditya-rana-6156071aa</v>
@@ -455,7 +455,7 @@
         <v>first</v>
       </c>
       <c r="C3" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="E3" t="str">
         <v>../members/armaan.webp</v>
@@ -484,7 +484,7 @@
         <v>first</v>
       </c>
       <c r="C4" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D4" t="str">
         <v>https://www.linkedin.com/in/chandan-kumar-19880a22a/</v>
@@ -516,7 +516,7 @@
         <v>first</v>
       </c>
       <c r="C5" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D5" t="str">
         <v>https://www.linkedin.com/in/charu-229665223</v>
@@ -548,7 +548,7 @@
         <v>first</v>
       </c>
       <c r="C6" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D6" t="str">
         <v>https://www.linkedin.com/in/dharuva-thakur-83576122a</v>
@@ -580,7 +580,7 @@
         <v>first</v>
       </c>
       <c r="C7" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D7" t="str">
         <v>https://www.linkedin.com/in/ekansh-verma-469557228</v>
@@ -612,7 +612,7 @@
         <v>first</v>
       </c>
       <c r="C8" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D8" t="str">
         <v>https://www.linkedin.com/in/gargi-dhawan-7706a722a</v>
@@ -644,7 +644,7 @@
         <v>first</v>
       </c>
       <c r="C9" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D9" t="str">
         <v>https://www.linkedin.com/in/hardik-sachdeva-a69987217</v>
@@ -676,7 +676,7 @@
         <v>first</v>
       </c>
       <c r="C10" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D10" t="str">
         <v>https://www.linkedin.com/in/jeevak-sangodkar-919653228/</v>
@@ -708,7 +708,7 @@
         <v>first</v>
       </c>
       <c r="C11" t="str">
-        <v>Volunteer  Member</v>
+        <v>Executive  Member</v>
       </c>
       <c r="D11" t="str">
         <v>https://www.linkedin.com/in/kanika-sharma-aa274b22a</v>
@@ -740,7 +740,7 @@
         <v>first</v>
       </c>
       <c r="C12" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="E12" t="str">
         <v>../members/kuldeep.webp</v>
@@ -769,7 +769,7 @@
         <v>first</v>
       </c>
       <c r="C13" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D13" t="str">
         <v>https://www.linkedin.com/in/madhukesh-singh-195618233/</v>
@@ -801,7 +801,7 @@
         <v>first</v>
       </c>
       <c r="C14" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="E14" t="str">
         <v>../members/manik.webp</v>
@@ -830,7 +830,7 @@
         <v>first</v>
       </c>
       <c r="C15" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D15" t="str">
         <v>https://www.linkedin.com/in/mehul-aggarwal-47285421b/</v>
@@ -862,7 +862,7 @@
         <v>first</v>
       </c>
       <c r="C16" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D16" t="str">
         <v>https://www.linkedin.com/in/navdeep-kaur-44375022a/</v>
@@ -894,10 +894,16 @@
         <v>first</v>
       </c>
       <c r="C17" t="str">
-        <v>Volenteer Member</v>
+        <v>Executive Member</v>
+      </c>
+      <c r="D17" t="str">
+        <v>https://www.linkedin.com/in/shashank-shekhar-196786229/</v>
       </c>
       <c r="E17" t="str">
         <v>../members/shashank.webp</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Material Science and Engineering</v>
       </c>
       <c r="H17" t="str">
         <v>Jamui</v>
@@ -917,7 +923,7 @@
         <v>first</v>
       </c>
       <c r="C18" t="str">
-        <v>Volunteer  Member</v>
+        <v>Executive  Member</v>
       </c>
       <c r="D18" t="str">
         <v>https://www.linkedin.com/in/shariq-verma-94a75122a</v>
@@ -949,7 +955,7 @@
         <v>first</v>
       </c>
       <c r="C19" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D19" t="str">
         <v>https://www.linkedin.com/in/siya-rana-b07639221</v>
@@ -981,7 +987,7 @@
         <v>first</v>
       </c>
       <c r="C20" t="str">
-        <v>Volunteer Member</v>
+        <v>Executive Member</v>
       </c>
       <c r="D20" t="str">
         <v>https://www.linkedin.com/in/swastkk</v>

</xml_diff>

<commit_message>
branch changed of Branch changers
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -905,7 +905,7 @@
         <v>../members/shashank.webp</v>
       </c>
       <c r="G17" t="str">
-        <v>Material Science and Engineering</v>
+        <v>Mechanical Engineering</v>
       </c>
       <c r="H17" t="str">
         <v>Jamui</v>
@@ -1001,7 +1001,7 @@
         <v>15p06FU4eSbaUxpU2A1mq4bD9BS5PxPxu</v>
       </c>
       <c r="G20" t="str">
-        <v>Civil Engineering</v>
+        <v>Electrical Engineering</v>
       </c>
       <c r="H20" t="str">
         <v>UNA</v>
@@ -1010,7 +1010,7 @@
         <v>Himachal Pradesh</v>
       </c>
       <c r="J20" t="str">
-        <v>A CE Undergrad at NIT Hamirpur currently learning new Web Technologies at Top pace.</v>
+        <v>A EE Undergrad at NIT Hamirpur currently learning new Web Technologies at Top pace.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sheet update for Ist year 2k22
Signed-off-by: swastik <swastkk@gmail.com>
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
-    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
-    <sheet r:id="rId3" sheetId="3" name="Sheet3"/>
-    <sheet r:id="rId4" sheetId="4" name="Sheet4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
+    <sheet name="sheet5" sheetId="5" r:id="rId7"/>
   </sheets>
+  <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="391">
   <si>
     <t>name</t>
   </si>
@@ -1123,20 +1125,99 @@
   </si>
   <si>
     <t>Electrical Sophomore at NIT Hamirpur currently learning new Web Technologies at Top pace.</t>
+  </si>
+  <si>
+    <t>img_link</t>
+  </si>
+  <si>
+    <t>Abhinamyu Singh</t>
+  </si>
+  <si>
+    <t>First Year</t>
+  </si>
+  <si>
+    <t>Aditya Sharma</t>
+  </si>
+  <si>
+    <t>Ankur Yadav</t>
+  </si>
+  <si>
+    <t>Anshuman Payasi</t>
+  </si>
+  <si>
+    <t>Archan Banerjee</t>
+  </si>
+  <si>
+    <t>Ayan Chadoria</t>
+  </si>
+  <si>
+    <t>Ayushi Shukla</t>
+  </si>
+  <si>
+    <t>Gugli Thakur</t>
+  </si>
+  <si>
+    <t>Kunal Dhiman</t>
+  </si>
+  <si>
+    <t>Laksh Bhandari</t>
+  </si>
+  <si>
+    <t>Mehul Ambastha</t>
+  </si>
+  <si>
+    <t>Naman Sharma</t>
+  </si>
+  <si>
+    <t>Oshin Sharma</t>
+  </si>
+  <si>
+    <t>Prikshit Saini</t>
+  </si>
+  <si>
+    <t>Rishika Sharma</t>
+  </si>
+  <si>
+    <t>Sakshi Gothwal</t>
+  </si>
+  <si>
+    <t>Sana Sheikh</t>
+  </si>
+  <si>
+    <t>Tanashvi Joshi</t>
+  </si>
+  <si>
+    <t>Urvashi Pandey</t>
+  </si>
+  <si>
+    <t>Vishesh Garg</t>
+  </si>
+  <si>
+    <t>Volunteer Member</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1156,26 +1237,127 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1186,10 +1368,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1465,29 +1647,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35fe5fd6-4564-4bb2-8bd0-89047bac716b}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1519,7 +1692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>286</v>
       </c>
@@ -1551,7 +1724,7 @@
         <v>292</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>293</v>
       </c>
@@ -1583,7 +1756,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>298</v>
       </c>
@@ -1615,7 +1788,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>302</v>
       </c>
@@ -1647,7 +1820,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>306</v>
       </c>
@@ -1679,7 +1852,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="40.5">
+    <row r="7" spans="1:10" ht="40.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>310</v>
       </c>
@@ -1711,7 +1884,7 @@
         <v>314</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>315</v>
       </c>
@@ -1743,7 +1916,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:10" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>319</v>
       </c>
@@ -1773,7 +1946,7 @@
         <v>324</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:10" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>325</v>
       </c>
@@ -1805,7 +1978,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:10" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>330</v>
       </c>
@@ -1837,7 +2010,7 @@
         <v>334</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:10" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>335</v>
       </c>
@@ -1869,7 +2042,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:10" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>338</v>
       </c>
@@ -1901,7 +2074,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:10" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>341</v>
       </c>
@@ -1933,7 +2106,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:10" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>344</v>
       </c>
@@ -1965,7 +2138,7 @@
         <v>347</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:10" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>348</v>
       </c>
@@ -1997,7 +2170,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:10" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>351</v>
       </c>
@@ -2027,7 +2200,7 @@
         <v>297</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" spans="1:10" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>355</v>
       </c>
@@ -2059,7 +2232,7 @@
         <v>358</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:10" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>359</v>
       </c>
@@ -2091,7 +2264,7 @@
         <v>362</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:10" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>363</v>
       </c>
@@ -2129,29 +2302,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29d399ae-7051-4559-9cb8-e0eac3c2848e}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>205</v>
       </c>
@@ -2215,7 +2379,7 @@
         <v>211</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>212</v>
       </c>
@@ -2247,7 +2411,7 @@
         <v>215</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>216</v>
       </c>
@@ -2277,7 +2441,7 @@
         <v>220</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>221</v>
       </c>
@@ -2309,7 +2473,7 @@
         <v>225</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>226</v>
       </c>
@@ -2341,7 +2505,7 @@
         <v>228</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:10" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>229</v>
       </c>
@@ -2373,7 +2537,7 @@
         <v>233</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>234</v>
       </c>
@@ -2405,7 +2569,7 @@
         <v>238</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:10" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>239</v>
       </c>
@@ -2437,7 +2601,7 @@
         <v>244</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:10" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>245</v>
       </c>
@@ -2469,7 +2633,7 @@
         <v>248</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:10" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>249</v>
       </c>
@@ -2501,7 +2665,7 @@
         <v>251</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:10" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>252</v>
       </c>
@@ -2533,7 +2697,7 @@
         <v>255</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:10" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>256</v>
       </c>
@@ -2565,7 +2729,7 @@
         <v>260</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:10" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>261</v>
       </c>
@@ -2597,7 +2761,7 @@
         <v>265</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:10" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>266</v>
       </c>
@@ -2629,7 +2793,7 @@
         <v>269</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:10" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>270</v>
       </c>
@@ -2661,7 +2825,7 @@
         <v>269</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:10" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>272</v>
       </c>
@@ -2693,7 +2857,7 @@
         <v>276</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" spans="1:10" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>277</v>
       </c>
@@ -2725,7 +2889,7 @@
         <v>281</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:10" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>282</v>
       </c>
@@ -2763,29 +2927,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73c3c79a-0418-4751-b5c0-501a8f9bbac3}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2817,7 +2972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
@@ -2849,7 +3004,7 @@
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>126</v>
       </c>
@@ -2881,7 +3036,7 @@
         <v>132</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>133</v>
       </c>
@@ -2913,7 +3068,7 @@
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
@@ -2945,7 +3100,7 @@
         <v>144</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>145</v>
       </c>
@@ -2977,7 +3132,7 @@
         <v>150</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:10" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>151</v>
       </c>
@@ -3009,7 +3164,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>157</v>
       </c>
@@ -3041,7 +3196,7 @@
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:10" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>164</v>
       </c>
@@ -3071,7 +3226,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:10" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>169</v>
       </c>
@@ -3103,7 +3258,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:10" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>174</v>
       </c>
@@ -3135,7 +3290,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:10" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>179</v>
       </c>
@@ -3165,7 +3320,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:10" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>183</v>
       </c>
@@ -3197,7 +3352,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:10" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>187</v>
       </c>
@@ -3227,7 +3382,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:10" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>191</v>
       </c>
@@ -3259,7 +3414,7 @@
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:10" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>196</v>
       </c>
@@ -3291,7 +3446,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:10" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>200</v>
       </c>
@@ -3329,29 +3484,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96ce9a20-80e1-458c-bcf8-c2eb72ec5dff}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3383,7 +3529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3415,7 +3561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -3447,7 +3593,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -3479,7 +3625,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -3511,7 +3657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -3543,7 +3689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:10" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -3575,7 +3721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -3607,7 +3753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:10" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
@@ -3639,7 +3785,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:10" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -3671,7 +3817,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:10" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>81</v>
       </c>
@@ -3703,7 +3849,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:10" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -3735,7 +3881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:10" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
@@ -3767,7 +3913,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:10" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>99</v>
       </c>
@@ -3797,7 +3943,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:10" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
@@ -3829,7 +3975,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:10" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>111</v>
       </c>
@@ -3864,4 +4010,292 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2525e50a-e2f2-4a31-ab24-43517b03ea62}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="3:3" ht="18.75" customHeight="1">
+      <c r="C28" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First year added 2k22
Signed-off-by: swastik <swastkk@gmail.com>
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
-    <sheet name="sheet5" sheetId="5" r:id="rId7"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet5"/>
+    <sheet r:id="rId2" sheetId="2" name="Sheet1"/>
+    <sheet r:id="rId3" sheetId="3" name="Sheet2"/>
+    <sheet r:id="rId4" sheetId="4" name="Sheet3"/>
+    <sheet r:id="rId5" sheetId="5" name="Sheet4"/>
   </sheets>
-  <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="414">
   <si>
     <t>name</t>
   </si>
@@ -882,7 +881,7 @@
     <t>Aditya Rana</t>
   </si>
   <si>
-    <t>first</t>
+    <t>Second</t>
   </si>
   <si>
     <t>Executive Member</t>
@@ -1136,71 +1135,141 @@
     <t>First Year</t>
   </si>
   <si>
+    <t>Volunteer Member</t>
+  </si>
+  <si>
+    <t>../members/abhimanyu.webp</t>
+  </si>
+  <si>
+    <t>______</t>
+  </si>
+  <si>
+    <t>_____</t>
+  </si>
+  <si>
     <t>Aditya Sharma</t>
   </si>
   <si>
+    <t>../members/adityasharma.webp</t>
+  </si>
+  <si>
     <t>Ankur Yadav</t>
   </si>
   <si>
+    <t>../members/ankur.webp</t>
+  </si>
+  <si>
     <t>Anshuman Payasi</t>
   </si>
   <si>
+    <t>../members/anshuman.webp</t>
+  </si>
+  <si>
     <t>Archan Banerjee</t>
   </si>
   <si>
+    <t xml:space="preserve">First </t>
+  </si>
+  <si>
+    <t>../members/archan.webp</t>
+  </si>
+  <si>
     <t>Ayan Chadoria</t>
   </si>
   <si>
+    <t>../members/ayan.webp</t>
+  </si>
+  <si>
     <t>Ayushi Shukla</t>
   </si>
   <si>
+    <t>../members/ayushishukla.webp</t>
+  </si>
+  <si>
     <t>Gugli Thakur</t>
   </si>
   <si>
+    <t>../members/gugli.webp</t>
+  </si>
+  <si>
     <t>Kunal Dhiman</t>
   </si>
   <si>
+    <t>../members/kunaldhiman.webp</t>
+  </si>
+  <si>
     <t>Laksh Bhandari</t>
   </si>
   <si>
+    <t>../members/laksh.webp</t>
+  </si>
+  <si>
     <t>Mehul Ambastha</t>
   </si>
   <si>
+    <t>../members/mehulambastha.webp</t>
+  </si>
+  <si>
     <t>Naman Sharma</t>
   </si>
   <si>
+    <t>../members/naman.webp</t>
+  </si>
+  <si>
     <t>Oshin Sharma</t>
   </si>
   <si>
+    <t>../members/oshin.webp</t>
+  </si>
+  <si>
     <t>Prikshit Saini</t>
   </si>
   <si>
+    <t>../members/prikshit.webp</t>
+  </si>
+  <si>
     <t>Rishika Sharma</t>
   </si>
   <si>
+    <t>../members/rishika.webp</t>
+  </si>
+  <si>
     <t>Sakshi Gothwal</t>
   </si>
   <si>
+    <t>../members/sakshi.webp</t>
+  </si>
+  <si>
     <t>Sana Sheikh</t>
   </si>
   <si>
+    <t>../members/sana.webp</t>
+  </si>
+  <si>
     <t>Tanashvi Joshi</t>
   </si>
   <si>
+    <t>../members/tenashvi.webp</t>
+  </si>
+  <si>
     <t>Urvashi Pandey</t>
   </si>
   <si>
+    <t>../members/urvashi.webp</t>
+  </si>
+  <si>
     <t>Vishesh Garg</t>
   </si>
   <si>
-    <t>Volunteer Member</t>
+    <t>../members/vishesh.webp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,13 +1278,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1228,7 +1298,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -1237,127 +1314,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-  </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1368,10 +1353,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1647,27 +1632,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35fe5fd6-4564-4bb2-8bd0-89047bac716b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1677,7 +1671,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>368</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -1692,608 +1686,604 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>286</v>
+        <v>369</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>288</v>
+        <v>370</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>371</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>289</v>
+        <v>181</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>294</v>
+        <v>181</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>296</v>
+        <v>373</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>299</v>
+        <v>181</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>50</v>
+        <v>373</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>301</v>
+        <v>373</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>373</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>303</v>
+        <v>181</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>305</v>
+        <v>373</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>259</v>
+        <v>373</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>307</v>
+        <v>181</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>143</v>
+        <v>373</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>259</v>
+        <v>373</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>311</v>
+        <v>181</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>149</v>
+        <v>373</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>313</v>
+        <v>373</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>316</v>
+        <v>181</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>373</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>131</v>
+        <v>373</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>318</v>
+        <v>373</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>320</v>
+        <v>181</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>321</v>
+        <v>389</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>322</v>
+        <v>373</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>323</v>
+        <v>373</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>326</v>
+        <v>181</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>328</v>
+        <v>373</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>329</v>
+        <v>373</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>331</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>332</v>
+        <v>181</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>149</v>
+        <v>373</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>336</v>
+        <v>181</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>124</v>
+        <v>373</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="A13" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>339</v>
+        <v>181</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>71</v>
+        <v>373</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>161</v>
+        <v>373</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>162</v>
+        <v>373</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="A14" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>342</v>
+        <v>181</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>373</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>259</v>
+        <v>373</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>345</v>
+        <v>181</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>242</v>
+        <v>373</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>323</v>
+        <v>373</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>349</v>
+        <v>181</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>108</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>137</v>
+        <v>373</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="A17" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>352</v>
+        <v>181</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>353</v>
+        <v>405</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>34</v>
+        <v>373</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>354</v>
+        <v>373</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>162</v>
+        <v>373</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>331</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>356</v>
+        <v>181</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>42</v>
+        <v>373</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>131</v>
+        <v>373</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>360</v>
+        <v>181</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>275</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>50</v>
+        <v>373</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>288</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+      <c r="A20" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>371</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>364</v>
+        <v>181</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>280</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>149</v>
+        <v>373</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>367</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+      <c r="A21" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -2302,20 +2292,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29d399ae-7051-4559-9cb8-e0eac3c2848e}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2347,578 +2346,608 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>208</v>
+        <v>289</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>209</v>
+        <v>290</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>293</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>213</v>
+        <v>294</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>214</v>
+        <v>295</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>296</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
-        <v>221</v>
+        <v>302</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>222</v>
+        <v>303</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>223</v>
+        <v>304</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>130</v>
+        <v>305</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>259</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
-        <v>226</v>
+        <v>306</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>181</v>
+        <v>307</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>227</v>
+        <v>308</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>309</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>27</v>
+        <v>259</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
-        <v>229</v>
+        <v>310</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>181</v>
+        <v>311</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>230</v>
+        <v>312</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>231</v>
+        <v>149</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1">
+        <v>314</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="1" t="s">
-        <v>234</v>
+        <v>315</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
+        <v>316</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>235</v>
+        <v>317</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>236</v>
+        <v>131</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>237</v>
+        <v>318</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="1" t="s">
-        <v>239</v>
+        <v>319</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>42</v>
+        <v>309</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>242</v>
+        <v>322</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>243</v>
+        <v>323</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17.25" customHeight="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="1" t="s">
-        <v>245</v>
+        <v>325</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>246</v>
+        <v>326</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>247</v>
+        <v>327</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>84</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>72</v>
+        <v>328</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>329</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="1" t="s">
-        <v>249</v>
+        <v>330</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>207</v>
+        <v>331</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>181</v>
+        <v>332</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>250</v>
+        <v>333</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1">
+        <v>334</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1" t="s">
-        <v>252</v>
+        <v>335</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>181</v>
+        <v>336</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>253</v>
+        <v>337</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>97</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>231</v>
+        <v>291</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>254</v>
+        <v>124</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1" t="s">
-        <v>256</v>
+        <v>338</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>257</v>
+        <v>339</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>258</v>
+        <v>340</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>102</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>149</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>232</v>
+        <v>161</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>259</v>
+        <v>162</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1" t="s">
-        <v>261</v>
+        <v>341</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>262</v>
+        <v>342</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>263</v>
+        <v>343</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>264</v>
+        <v>204</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1" t="s">
-        <v>266</v>
+        <v>344</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>267</v>
+        <v>345</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>25</v>
+        <v>291</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17.25" customHeight="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F17" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>285</v>
+        <v>362</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+      <c r="A20" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -2927,20 +2956,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73c3c79a-0418-4751-b5c0-501a8f9bbac3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2972,281 +3010,281 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>121</v>
+        <v>207</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>122</v>
+        <v>208</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>123</v>
+        <v>209</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>210</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>212</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>207</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>131</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
-        <v>133</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>135</v>
+        <v>217</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>136</v>
+        <v>218</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>142</v>
+        <v>223</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>243</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17.25" customHeight="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>245</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>171</v>
+        <v>246</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>172</v>
+        <v>247</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>72</v>
@@ -3255,30 +3293,30 @@
         <v>36</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" customHeight="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="1" t="s">
-        <v>174</v>
+        <v>249</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>177</v>
+        <v>250</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>210</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>109</v>
@@ -3287,195 +3325,263 @@
         <v>27</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1" t="s">
-        <v>179</v>
+        <v>252</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>182</v>
+        <v>253</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>254</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17.25" customHeight="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>186</v>
+        <v>258</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="A14" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="J15" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1">
+        <v>269</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>270</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>199</v>
+        <v>271</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17.25" customHeight="1">
+        <v>269</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1" t="s">
-        <v>200</v>
+        <v>272</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>201</v>
+        <v>273</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>204</v>
+        <v>51</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>156</v>
+        <v>276</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3484,20 +3590,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96ce9a20-80e1-458c-bcf8-c2eb72ec5dff}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="12.428571428571429" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="49.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3529,482 +3644,510 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>152</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>159</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17.25" customHeight="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="1" t="s">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>77</v>
+        <v>172</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17.25" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>187</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>188</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>190</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>102</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17.25" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>193</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1">
+        <v>195</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>196</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>112</v>
+        <v>197</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>118</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="A17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4013,289 +4156,539 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2525e50a-e2f2-4a31-ab24-43517b03ea62}">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>368</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15">
-      <c r="A2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C28" s="3"/>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="A14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add First year details
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="460">
   <si>
     <t>name</t>
   </si>
@@ -1141,10 +1141,13 @@
     <t>../members/abhimanyu.webp</t>
   </si>
   <si>
-    <t>______</t>
-  </si>
-  <si>
-    <t>_____</t>
+    <t>CSE dual</t>
+  </si>
+  <si>
+    <t>Bareilly</t>
+  </si>
+  <si>
+    <t>I'm a go getter kind of person.Presently, exploring different tech domains and trying to inculcate them in myself.</t>
   </si>
   <si>
     <t>Aditya Sharma</t>
@@ -1153,18 +1156,40 @@
     <t>../members/adityasharma.webp</t>
   </si>
   <si>
+    <t>Trying to Grab as many opportunities as I can.Learning to grow. Finance,Design and Tech</t>
+  </si>
+  <si>
     <t>Ankur Yadav</t>
   </si>
   <si>
     <t>../members/ankur.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Mathematics and Computing </t>
+  </si>
+  <si>
+    <t>Love to Write. Tech and PR. An extrovert with an introvert's soul.</t>
+  </si>
+  <si>
     <t>Anshuman Payasi</t>
   </si>
   <si>
     <t>../members/anshuman.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Electrical Engineering </t>
+  </si>
+  <si>
+    <t>Rewa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madhya Pradesh </t>
+  </si>
+  <si>
+    <t>Exploring various fields, learning, and implementing new ideas into practice.
+Field of interest are programming, designing, video editing, sports, photography, gaming.</t>
+  </si>
+  <si>
     <t>Archan Banerjee</t>
   </si>
   <si>
@@ -1174,94 +1199,208 @@
     <t>../members/archan.webp</t>
   </si>
   <si>
+    <t>Engineering Physics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asansol </t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>Wandering in the valleys of Coding languages while surfing against the Waves of Data and Bugs.Ambivert</t>
+  </si>
+  <si>
     <t>Ayan Chadoria</t>
   </si>
   <si>
     <t>../members/ayan.webp</t>
   </si>
   <si>
+    <t>Jodhpur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating bugs is my passion and Writing poems is my hobby. I'm a tech geek who writes, codes, invests, sleeps, and eats.exploring both the world and new technologies. </t>
+  </si>
+  <si>
     <t>Ayushi Shukla</t>
   </si>
   <si>
     <t>../members/ayushishukla.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Mechanical engineering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uttar Pradesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inquisitive and enthusiastic about exploring new domains to find my passion! </t>
+  </si>
+  <si>
     <t>Gugli Thakur</t>
   </si>
   <si>
     <t>../members/gugli.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil Engineering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring my capabilities to mix up in this world </t>
+  </si>
+  <si>
     <t>Kunal Dhiman</t>
   </si>
   <si>
     <t>../members/kunaldhiman.webp</t>
   </si>
   <si>
+    <t>Dual CSE</t>
+  </si>
+  <si>
+    <t>Learning web developement</t>
+  </si>
+  <si>
     <t>Laksh Bhandari</t>
   </si>
   <si>
     <t>../members/laksh.webp</t>
   </si>
   <si>
+    <t>Haldwani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uttarakhand </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An amateur boy who likes to capture beautiful moments of his life. </t>
+  </si>
+  <si>
     <t>Mehul Ambastha</t>
   </si>
   <si>
     <t>../members/mehulambastha.webp</t>
   </si>
   <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>The guy with quick witty replies. Knows tech but can't draw a freehand circle. Passionate about PR and Technical domains whilst exploring everything that comes my way!</t>
+  </si>
+  <si>
     <t>Naman Sharma</t>
   </si>
   <si>
     <t>../members/naman.webp</t>
   </si>
   <si>
+    <t>Panipat</t>
+  </si>
+  <si>
+    <t>Exploring every bit of life and learning as much as i can</t>
+  </si>
+  <si>
     <t>Oshin Sharma</t>
   </si>
   <si>
     <t>../members/oshin.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Electronics and Communication Engineering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una </t>
+  </si>
+  <si>
+    <t>Embracing the roller-coaster of life whilst finding joy in the journey and strength in the struggle.</t>
+  </si>
+  <si>
     <t>Prikshit Saini</t>
   </si>
   <si>
     <t>../members/prikshit.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Computer Science and Engineering </t>
+  </si>
+  <si>
+    <t>Baddi</t>
+  </si>
+  <si>
+    <t>A tech enthusiast keen in exploring new things and trying to unleash the true power of myself.</t>
+  </si>
+  <si>
     <t>Rishika Sharma</t>
   </si>
   <si>
     <t>../members/rishika.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Material Science and Engineering </t>
+  </si>
+  <si>
+    <t>I believe in constantly challenging myself to grow and learn, and I am not afraid of hard work and perseverance to reach my goals</t>
+  </si>
+  <si>
     <t>Sakshi Gothwal</t>
   </si>
   <si>
     <t>../members/sakshi.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Rajasthan </t>
+  </si>
+  <si>
+    <t>I enjoy exploring new ideas and finding new ways to bring my visions to life.</t>
+  </si>
+  <si>
     <t>Sana Sheikh</t>
   </si>
   <si>
     <t>../members/sana.webp</t>
   </si>
   <si>
+    <t>As an optimistic and effervescent personality, I try to explore as much of myself as I can and try to put in my best in everything I do in all the fields.</t>
+  </si>
+  <si>
     <t>Tanashvi Joshi</t>
   </si>
   <si>
     <t>../members/tenashvi.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">Engineering Physics </t>
+  </si>
+  <si>
+    <t>Barabanki</t>
+  </si>
+  <si>
+    <t>Enthusiastic Human.Tends to turn the flow of life in the direction I wish.</t>
+  </si>
+  <si>
     <t>Urvashi Pandey</t>
   </si>
   <si>
     <t>../members/urvashi.webp</t>
   </si>
   <si>
+    <t>Gorakhpur</t>
+  </si>
+  <si>
+    <t>still searchin' me within myself!</t>
+  </si>
+  <si>
     <t>Vishesh Garg</t>
   </si>
   <si>
     <t>../members/vishesh.webp</t>
+  </si>
+  <si>
+    <t>Ghaziabad</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1269,7 +1408,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1279,7 +1418,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1287,6 +1426,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1317,7 +1462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1325,11 +1470,20 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1642,26 +1796,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="32.86214285714286" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="26.14785714285714" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1686,14 +1840,14 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>371</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1707,583 +1861,583 @@
         <v>373</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>373</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>373</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>373</v>
+        <v>242</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>373</v>
+        <v>124</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>373</v>
+        <v>259</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="34.5">
+      <c r="A5" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>374</v>
+        <v>387</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>388</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>373</v>
+        <v>392</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>373</v>
+        <v>394</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>374</v>
+        <v>395</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>373</v>
+        <v>149</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>373</v>
+        <v>80</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>373</v>
+        <v>402</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>373</v>
+        <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>373</v>
+        <v>403</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>374</v>
+        <v>404</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>373</v>
+        <v>143</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>373</v>
+        <v>259</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>391</v>
+        <v>410</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>373</v>
+        <v>411</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>373</v>
+        <v>51</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>373</v>
+        <v>27</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>374</v>
+        <v>412</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>393</v>
+        <v>414</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>373</v>
+        <v>296</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>373</v>
+        <v>415</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>373</v>
+        <v>402</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>373</v>
+        <v>420</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>373</v>
+        <v>420</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>374</v>
+        <v>421</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>397</v>
+        <v>423</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>373</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>373</v>
+        <v>424</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>373</v>
+        <v>18</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>374</v>
+        <v>425</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>399</v>
+        <v>427</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>373</v>
+        <v>428</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>373</v>
+        <v>429</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>373</v>
+        <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>401</v>
+        <v>432</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>373</v>
+        <v>433</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>373</v>
+        <v>434</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>373</v>
+        <v>27</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>374</v>
+        <v>435</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>403</v>
+        <v>437</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>373</v>
+        <v>438</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>373</v>
+        <v>80</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>374</v>
+        <v>439</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>405</v>
+        <v>441</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>373</v>
+        <v>433</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>373</v>
+        <v>79</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>373</v>
+        <v>442</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>374</v>
+        <v>443</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="A18" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>407</v>
+        <v>445</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>373</v>
+        <v>131</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>373</v>
+        <v>27</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>374</v>
+        <v>446</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>373</v>
+        <v>449</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>373</v>
+        <v>450</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>373</v>
+        <v>36</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>374</v>
+        <v>451</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>411</v>
+        <v>453</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>373</v>
+        <v>454</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>373</v>
+        <v>403</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>374</v>
+        <v>455</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>413</v>
+        <v>457</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>373</v>
+        <v>458</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>374</v>
+        <v>403</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor nits in links fixed
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="477">
   <si>
     <t>name</t>
   </si>
@@ -1138,6 +1138,9 @@
     <t>Volunteer Member</t>
   </si>
   <si>
+    <t>http://linkedin.com/in/abhimanyu-singh-326343266</t>
+  </si>
+  <si>
     <t>../members/abhimanyu.webp</t>
   </si>
   <si>
@@ -1153,6 +1156,9 @@
     <t>Aditya Sharma</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/aditya-sharma-82997921b</t>
+  </si>
+  <si>
     <t>../members/adityasharma.webp</t>
   </si>
   <si>
@@ -1162,6 +1168,9 @@
     <t>Ankur Yadav</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/ankuryadavsolan</t>
+  </si>
+  <si>
     <t>../members/ankur.webp</t>
   </si>
   <si>
@@ -1172,6 +1181,9 @@
   </si>
   <si>
     <t>Anshuman Payasi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/anshumanpayasi</t>
   </si>
   <si>
     <t>../members/anshuman.webp</t>
@@ -1196,6 +1208,9 @@
     <t xml:space="preserve">First </t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>../members/archan.webp</t>
   </si>
   <si>
@@ -1214,6 +1229,9 @@
     <t>Ayan Chadoria</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/ayanchoradia</t>
+  </si>
+  <si>
     <t>../members/ayan.webp</t>
   </si>
   <si>
@@ -1226,6 +1244,9 @@
     <t>Ayushi Shukla</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/ayushi-shukla-7498b125b</t>
+  </si>
+  <si>
     <t>../members/ayushishukla.webp</t>
   </si>
   <si>
@@ -1241,6 +1262,9 @@
     <t>Gugli Thakur</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/gugli-thakur-73479425b</t>
+  </si>
+  <si>
     <t>../members/gugli.webp</t>
   </si>
   <si>
@@ -1265,6 +1289,9 @@
     <t>Laksh Bhandari</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/laksh-bhandari-70a4b225b</t>
+  </si>
+  <si>
     <t>../members/laksh.webp</t>
   </si>
   <si>
@@ -1292,6 +1319,9 @@
     <t>Naman Sharma</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/naman-sharma-7928a1223</t>
+  </si>
+  <si>
     <t>../members/naman.webp</t>
   </si>
   <si>
@@ -1304,6 +1334,9 @@
     <t>Oshin Sharma</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/oshin-sharma-b22584257</t>
+  </si>
+  <si>
     <t>../members/oshin.webp</t>
   </si>
   <si>
@@ -1319,6 +1352,9 @@
     <t>Prikshit Saini</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/prikshit-saini-1276a325b</t>
+  </si>
+  <si>
     <t>../members/prikshit.webp</t>
   </si>
   <si>
@@ -1334,6 +1370,9 @@
     <t>Rishika Sharma</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/rishika-sharma-5bb235258</t>
+  </si>
+  <si>
     <t>../members/rishika.webp</t>
   </si>
   <si>
@@ -1346,6 +1385,9 @@
     <t>Sakshi Gothwal</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/sakshi-gothwal-0466a925a</t>
+  </si>
+  <si>
     <t>../members/sakshi.webp</t>
   </si>
   <si>
@@ -1358,6 +1400,9 @@
     <t>Sana Sheikh</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/sana-sheikh-a24714257</t>
+  </si>
+  <si>
     <t>../members/sana.webp</t>
   </si>
   <si>
@@ -1367,6 +1412,9 @@
     <t>Tanashvi Joshi</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/tanashvi-joshi-528412255</t>
+  </si>
+  <si>
     <t>../members/tenashvi.webp</t>
   </si>
   <si>
@@ -1382,6 +1430,9 @@
     <t>Urvashi Pandey</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/urvii-pandey-943021258</t>
+  </si>
+  <si>
     <t>../members/urvashi.webp</t>
   </si>
   <si>
@@ -1394,13 +1445,13 @@
     <t>Vishesh Garg</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/vishesh-garg-140440258</t>
+  </si>
+  <si>
     <t>../members/vishesh.webp</t>
   </si>
   <si>
     <t>Ghaziabad</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -1799,7 +1850,7 @@
     <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="34.71928571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="32.86214285714286" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="26.14785714285714" customWidth="1" bestFit="1"/>
@@ -1851,28 +1902,28 @@
         <v>371</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>181</v>
+        <v>372</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>370</v>
@@ -1881,10 +1932,10 @@
         <v>371</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>181</v>
+        <v>378</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -1897,12 +1948,12 @@
         <v>323</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="5" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>370</v>
@@ -1911,14 +1962,14 @@
         <v>371</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>181</v>
+        <v>382</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>124</v>
@@ -1927,12 +1978,12 @@
         <v>259</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="34.5">
       <c r="A5" s="5" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>370</v>
@@ -1941,134 +1992,134 @@
         <v>371</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>387</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="5" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>181</v>
+      <c r="D6" s="7" t="s">
+        <v>395</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="5" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>181</v>
+        <v>402</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
         <v>149</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="5" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
+        <v>407</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="5" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>181</v>
+        <v>413</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>143</v>
@@ -2077,28 +2128,28 @@
         <v>259</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="5" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>181</v>
+      <c r="D10" s="7" t="s">
+        <v>395</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>51</v>
@@ -2107,238 +2158,238 @@
         <v>27</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="5" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>181</v>
+        <v>422</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>296</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="5" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>181</v>
+      <c r="D12" s="7" t="s">
+        <v>395</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="5" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>181</v>
+        <v>432</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="5" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>181</v>
+        <v>437</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="5" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>181</v>
+        <v>443</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="5" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>181</v>
+        <v>449</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="5" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>181</v>
+        <v>454</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>443</v>
+        <v>457</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="5" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>181</v>
+        <v>459</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>131</v>
@@ -2347,97 +2398,97 @@
         <v>27</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>446</v>
+        <v>461</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="5" t="s">
-        <v>447</v>
+        <v>462</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>181</v>
+        <v>463</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>448</v>
+        <v>464</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="5" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>181</v>
+        <v>469</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>454</v>
+        <v>471</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>455</v>
+        <v>472</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="5" t="s">
-        <v>456</v>
+        <v>473</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>181</v>
+        <v>474</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>458</v>
+        <v>476</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>459</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -2459,7 +2510,7 @@
     <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="41.29071428571429" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
@@ -3123,7 +3174,7 @@
     <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="39.14785714285715" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>

</xml_diff>

<commit_message>
Sumit sir pic updated
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
@@ -595,7 +595,7 @@
     <t>https://www.linkedin.com/in/sumit-dhiman-20bce091</t>
   </si>
   <si>
-    <t>../members/Sumit2.webp</t>
+    <t>../members/sumit.webp</t>
   </si>
   <si>
     <t>1K4LpZE6yPe1EAsxK6zL7RwGDRhvTk97t</t>
@@ -1221,7 +1221,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1233,12 +1233,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -1281,18 +1275,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1302,9 +1296,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1631,10 +1622,10 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1693,13 +1684,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1723,13 +1714,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1753,13 +1744,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="34.5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1778,18 +1769,18 @@
       <c r="I5" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>312</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D6" s="3"/>
@@ -1811,13 +1802,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1841,13 +1832,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1871,13 +1862,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1901,13 +1892,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D10" s="3"/>
@@ -1929,13 +1920,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1959,13 +1950,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D12" s="3"/>
@@ -1987,13 +1978,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2017,13 +2008,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -2047,13 +2038,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2077,13 +2068,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -2107,13 +2098,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -2137,13 +2128,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -2167,13 +2158,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -2197,13 +2188,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -2227,13 +2218,13 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>290</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -3038,7 +3029,7 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3744,7 +3735,7 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3760,7 +3751,7 @@
     <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4382,7 +4373,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>

</xml_diff>

<commit_message>
Sheets updated for instagram of members
Signed-off-by: Swastik Sharma <swastkk@gmail.com>
</commit_message>
<xml_diff>
--- a/content/sheets/members.xlsx
+++ b/content/sheets/members.xlsx
@@ -35,8 +35,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -67,8 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,2407 +402,2635 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>year</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>description</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" s="1" t="str">
         <v>link</v>
       </c>
-      <c r="E1" t="str">
+      <c r="E1" s="1" t="str">
+        <v>insta</v>
+      </c>
+      <c r="F1" s="1" t="str">
         <v>img</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" s="1" t="str">
         <v>img_link</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" s="1" t="str">
         <v>branch</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" s="1" t="str">
         <v>city</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" s="1" t="str">
         <v>state</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" s="1" t="str">
         <v>about</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>Abhinamyu Singh</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="1" t="str">
         <v>First</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" s="1" t="str">
         <v>http://linkedin.com/in/abhimanyu-singh-326343266</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E2" s="1" t="str">
+        <v>https://instagram.com/alternate_manyu?igshid=YmMyMTA2M2Y=</v>
+      </c>
+      <c r="F2" s="1" t="str">
         <v>../members/abhimanyu.webp</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" s="1" t="str">
         <v>CSE dual</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" s="1" t="str">
         <v>Bareilly</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" s="1" t="str">
         <v>I'm a go getter kind of person.Presently, exploring different tech domains and trying to inculcate them in myself.</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <v>Aditya Sharma</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
         <v>https://www.linkedin.com/in/aditya-sharma-82997921b</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" s="1" t="str">
+        <v>https://instagram.com/_.adityasharma_._?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F3" s="1" t="str">
         <v>../members/adityasharma.webp</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" s="1" t="str">
         <v>Chemical Engineering</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" s="1" t="str">
         <v>Haridwar</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" s="1" t="str">
         <v>Uttarakhand</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" s="1" t="str">
         <v>Trying to Grab as many opportunities as I can.Learning to grow. Finance,Design and Tech</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" s="1" t="str">
         <v>Ankur Yadav</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="1" t="str">
         <v>First</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" s="1" t="str">
         <v>https://www.linkedin.com/in/ankuryadavsolan</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" s="1" t="str">
+        <v>https://instagram.com/ig_ankuryadav?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F4" s="1" t="str">
         <v>../members/ankur.webp</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" s="1" t="str">
         <v xml:space="preserve">Mathematics and Computing </v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" s="1" t="str">
         <v>Solan</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" s="1" t="str">
         <v>Love to Write. Tech and PR. An extrovert with an introvert's soul.</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
+      <c r="A5" s="1" t="str">
         <v>Anshuman Payasi</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="1" t="str">
         <v>First</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="1" t="str">
         <v>https://www.linkedin.com/in/anshumanpayasi</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="1" t="str">
+        <v>https://instagram.com/anshumaaaan_?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <v>../members/anshuman.webp</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" s="1" t="str">
         <v xml:space="preserve">Electrical Engineering </v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" s="1" t="str">
         <v>Rewa</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" s="1" t="str">
         <v xml:space="preserve">Madhya Pradesh </v>
       </c>
-      <c r="J5" t="str" xml:space="preserve">
+      <c r="K5" s="1" t="str" xml:space="preserve">
         <v xml:space="preserve">Exploring various fields, learning, and implementing new ideas into practice.
 Field of interest are programming, designing, video editing, sports, photography, gaming.</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <v>Archan Banerjee</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="1" t="str">
+        <v>https://instagram.com/_.g.o.o.f.y._?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <v>../members/archan.webp</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" s="1" t="str">
         <v>Engineering Physics</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" s="1" t="str">
         <v xml:space="preserve">Asansol </v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" s="1" t="str">
         <v>West Bengal</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" s="1" t="str">
         <v>Wandering in the valleys of Coding languages while surfing against the Waves of Data and Bugs.Ambivert</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
+      <c r="A7" s="1" t="str">
         <v>Ayan Chadoria</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" s="1" t="str">
         <v>https://www.linkedin.com/in/ayanchoradia</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="1" t="str">
+        <v>https://instagram.com/ayanchoradia?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <v>../members/ayan.webp</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" s="1" t="str">
         <v>Jodhpur</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" s="1" t="str">
         <v>Rajasthan</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" s="1" t="str">
         <v xml:space="preserve">Creating bugs is my passion and Writing poems is my hobby. I'm a tech geek who writes, codes, invests, sleeps, and eats.exploring both the world and new technologies. </v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
+      <c r="A8" s="1" t="str">
         <v>Ayushi Shukla</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" s="1" t="str">
         <v>https://www.linkedin.com/in/ayushi-shukla-7498b125b</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="1" t="str">
+        <v>https://instagram.com/ayushii_05_?igshid=NmQ2ZmYxZjA=</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <v>../members/ayushishukla.webp</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" s="1" t="str">
         <v xml:space="preserve">Mechanical engineering </v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" s="1" t="str">
         <v>Lucknow</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" s="1" t="str">
         <v xml:space="preserve">Uttar Pradesh </v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" s="1" t="str">
         <v xml:space="preserve">Inquisitive and enthusiastic about exploring new domains to find my passion! </v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
+      <c r="A9" s="1" t="str">
         <v>Gugli Thakur</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="1" t="str">
         <v>https://www.linkedin.com/in/gugli-thakur-73479425b</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="1" t="str">
+        <v>https://instagram.com/dude_its.gugli?igshid=NTE5MzUyOTU=</v>
+      </c>
+      <c r="F9" s="1" t="str">
         <v>../members/gugli.webp</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" s="1" t="str">
         <v xml:space="preserve">Civil Engineering </v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" s="1" t="str">
         <v>Mandi</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" s="1" t="str">
         <v xml:space="preserve">Exploring my capabilities to mix up in this world </v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
+      <c r="A10" s="1" t="str">
         <v>Kunal Dhiman</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="1" t="str">
+        <v>https://instagram.com/kunal_dhiman27971</v>
+      </c>
+      <c r="F10" s="1" t="str">
         <v>../members/kunaldhiman.webp</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" s="1" t="str">
         <v>Dual CSE</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" s="1" t="str">
         <v>Hamirpur</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" s="1" t="str">
         <v>Learning web developement</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
+      <c r="A11" s="1" t="str">
         <v>Laksh Bhandari</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="1" t="str">
         <v>https://www.linkedin.com/in/laksh-bhandari-70a4b225b</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="1" t="str">
+        <v>https://instagram.com/bhandari_g.29</v>
+      </c>
+      <c r="F11" s="1" t="str">
         <v>../members/laksh.webp</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" s="1" t="str">
         <v>Mathematics and Computing</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" s="1" t="str">
         <v>Haldwani</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" s="1" t="str">
         <v xml:space="preserve">Uttarakhand </v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" s="1" t="str">
         <v xml:space="preserve">An amateur boy who likes to capture beautiful moments of his life. </v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
+      <c r="A12" s="1" t="str">
         <v>Mehul Ambastha</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12" s="1" t="str">
+        <v>https://instagram.com/a.gyaani.ladka?igshid=YmMyMTA2M2Y=</v>
+      </c>
+      <c r="F12" s="1" t="str">
         <v>../members/mehulambastha.webp</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" s="1" t="str">
         <v xml:space="preserve">Mechanical engineering </v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" s="1" t="str">
         <v>Delhi</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" s="1" t="str">
         <v>Delhi</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" s="1" t="str">
         <v>The guy with quick witty replies. Knows tech but can't draw a freehand circle. Passionate about PR and Technical domains whilst exploring everything that comes my way!</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
+      <c r="A13" s="1" t="str">
         <v>Naman Sharma</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" s="1" t="str">
         <v>https://www.linkedin.com/in/naman-sharma-7928a1223</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E13" s="1" t="str">
+        <v>https://instagram.com/naman2236s?igshid=YmMyMTA2M2Y=</v>
+      </c>
+      <c r="F13" s="1" t="str">
         <v>../members/naman.webp</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" s="1" t="str">
         <v>Electronics and Communication Engineering</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" s="1" t="str">
         <v>Panipat</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" s="1" t="str">
         <v>Haryana</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" s="1" t="str">
         <v>Exploring every bit of life and learning as much as i can</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
+      <c r="A14" s="1" t="str">
         <v>Oshin Sharma</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14" s="1" t="str">
         <v>https://www.linkedin.com/in/oshin-sharma-b22584257</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E14" s="1" t="str">
+        <v>https://instagram.com/ohhshinnn?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F14" s="1" t="str">
         <v>../members/oshin.webp</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" s="1" t="str">
         <v xml:space="preserve">Electronics and Communication Engineering </v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" s="1" t="str">
         <v xml:space="preserve">Una </v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" s="1" t="str">
         <v>Embracing the roller-coaster of life whilst finding joy in the journey and strength in the struggle.</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
+      <c r="A15" s="1" t="str">
         <v>Prikshit Saini</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" s="1" t="str">
         <v>https://www.linkedin.com/in/prikshit-saini-1276a325b</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E15" s="1" t="str">
+        <v>https://www.instagram.com/invites/contact/?i=1dhjsr58wjn08&amp;utm_content=qf87blc</v>
+      </c>
+      <c r="F15" s="1" t="str">
         <v>../members/prikshit.webp</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" s="1" t="str">
         <v xml:space="preserve">Computer Science and Engineering </v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" s="1" t="str">
         <v>Baddi</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J15" t="str">
+      <c r="K15" s="1" t="str">
         <v>A tech enthusiast keen in exploring new things and trying to unleash the true power of myself.</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
+      <c r="A16" s="1" t="str">
         <v>Rishika Sharma</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" s="1" t="str">
         <v>https://www.linkedin.com/in/rishika-sharma-5bb235258</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E16" s="1" t="str">
+        <v>https://instagram.com/rishika07.__?igshid=NmQ2ZmYxZjA=</v>
+      </c>
+      <c r="F16" s="1" t="str">
         <v>../members/rishika.webp</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" s="1" t="str">
         <v xml:space="preserve">Material Science and Engineering </v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" s="1" t="str">
         <v>Jodhpur</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" s="1" t="str">
         <v>Rajasthan</v>
       </c>
-      <c r="J16" t="str">
+      <c r="K16" s="1" t="str">
         <v>I believe in constantly challenging myself to grow and learn, and I am not afraid of hard work and perseverance to reach my goals</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
+      <c r="A17" s="1" t="str">
         <v>Sakshi Gothwal</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="1" t="str">
         <v>https://www.linkedin.com/in/sakshi-gothwal-0466a925a</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="1" t="str">
+        <v>https://instagram.com/sakshi.gothwal?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F17" s="1" t="str">
         <v>../members/sakshi.webp</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" s="1" t="str">
         <v xml:space="preserve">Computer Science and Engineering </v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" s="1" t="str">
         <v>Jaipur</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" s="1" t="str">
         <v xml:space="preserve">Rajasthan </v>
       </c>
-      <c r="J17" t="str">
+      <c r="K17" s="1" t="str">
         <v>I enjoy exploring new ideas and finding new ways to bring my visions to life.</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
+      <c r="A18" s="1" t="str">
         <v>Sana Sheikh</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18" s="1" t="str">
         <v>https://www.linkedin.com/in/sana-sheikh-a24714257</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E18" s="1" t="str">
+        <v>https://instagram.com/_blu.aesthetics_?igshid=OGQ2MjdiOTE=</v>
+      </c>
+      <c r="F18" s="1" t="str">
         <v>../members/sana.webp</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" s="1" t="str">
         <v xml:space="preserve">Mathematics and Computing </v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" s="1" t="str">
         <v>Shimla</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J18" t="str">
+      <c r="K18" s="1" t="str">
         <v>As an optimistic and effervescent personality, I try to explore as much of myself as I can and try to put in my best in everything I do in all the fields.</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
+      <c r="A19" s="1" t="str">
         <v>Tanashvi Joshi</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19" s="1" t="str">
         <v>https://www.linkedin.com/in/tanashvi-joshi-528412255</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E19" s="1" t="str">
+        <v>https://instagram.com/tanashvi_joshi19?igshid=ZDdkNTZiNTM=</v>
+      </c>
+      <c r="F19" s="1" t="str">
         <v>../members/tenashvi.webp</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" s="1" t="str">
         <v xml:space="preserve">Engineering Physics </v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" s="1" t="str">
         <v>Barabanki</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J19" t="str">
+      <c r="K19" s="1" t="str">
         <v>Enthusiastic Human.Tends to turn the flow of life in the direction I wish.</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="str">
+      <c r="A20" s="1" t="str">
         <v>Urvashi Pandey</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="1" t="str">
         <v xml:space="preserve">First </v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="1" t="str">
         <v>Volunteer Member</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D20" s="1" t="str">
         <v>https://www.linkedin.com/in/urvii-pandey-943021258</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E20" s="1" t="str">
+        <v>https://instagram.com/urv_ssii.07?igshid=NmQ2ZmYxZjA=</v>
+      </c>
+      <c r="F20" s="1" t="str">
         <v>../members/urvashi.webp</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" s="1" t="str">
         <v xml:space="preserve">Civil Engineering </v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" s="1" t="str">
         <v>Gorakhpur</v>
       </c>
-      <c r="I20" t="str">
+      <c r="J20" s="1" t="str">
         <v xml:space="preserve">Uttar Pradesh </v>
       </c>
-      <c r="J20" t="str">
+      <c r="K20" s="1" t="str">
         <v>still searchin' me within myself!</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K20"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>year</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>description</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" s="1" t="str">
         <v>link</v>
       </c>
-      <c r="E1" t="str">
+      <c r="E1" s="1" t="str">
+        <v>insta</v>
+      </c>
+      <c r="F1" s="1" t="str">
         <v>img</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" s="1" t="str">
         <v>image_link</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" s="1" t="str">
         <v>branch</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" s="1" t="str">
         <v>city</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" s="1" t="str">
         <v>state</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" s="1" t="str">
         <v>about</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>Aditya Rana</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" s="1" t="str">
         <v>https://www.linkedin.com/in/aditya-rana-6156071aa</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E2" s="1" t="str">
+        <v>https://www.instagram.com/adt.rana/</v>
+      </c>
+      <c r="F2" s="1" t="str">
         <v>../members/aditiya.webp</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" s="1" t="str">
         <v>1LjuDNVhaQmaOaujbP3XWpNtAaXtnAZNo</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" s="1" t="str">
         <v>Computer science and Engineering</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" s="1" t="str">
         <v>I am an instance of my own class | Fresher @ CSE NITH | Always learning and implementing latest and greatest technologies | Freelancer @ fiverr | Android Developer |</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <v>Armaan Shukla</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
         <v>https://www.linkedin.com/in/armaan-shukla-b17a80141/</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" s="1" t="str">
+        <v>https://www.instagram.com/armaan._shukla/</v>
+      </c>
+      <c r="F3" s="1" t="str">
         <v>../members/armaan.webp</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" s="1" t="str">
         <v>1Tpnk2k0ZIv73FWy7JeLxcRBjC_Oq7O-f</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" s="1" t="str">
         <v>Mathematics and Computing</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" s="1" t="str">
         <v>Chandan Kumar</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" s="1" t="str">
         <v>https://www.linkedin.com/in/chandan-kumar-19880a22a/</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" s="1" t="str">
+        <v>https://www.instagram.com/chandan_._kr/</v>
+      </c>
+      <c r="F4" s="1" t="str">
         <v>../members/chandan.webp</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" s="1" t="str">
         <v>1522oz7z6THBgb0FxF4DmHlyI3YQpviNM</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" s="1" t="str">
         <v>Electronics and Communication Engineering</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" s="1" t="str">
         <v>Varanasi</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5" s="1" t="str">
         <v>Charu</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="1" t="str">
         <v>https://www.linkedin.com/in/charu-229665223</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="1" t="str">
+        <v>https://www.instagram.com/charuchauhan575/</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <v>../members/charu.webp</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" s="1" t="str">
         <v>1gYhb-XoUU6OsD2Zrk-eqEUR94UtYotqJ</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" s="1" t="str">
         <v xml:space="preserve">Mechanical Engineering </v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <v xml:space="preserve">Dharuva Thakur </v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="1" t="str">
         <v>https://www.linkedin.com/in/dharuva-thakur-83576122a</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="1" t="str">
+        <v>https://www.instagram.com/dharuva_thakur/</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <v>../members/dharuva.webp</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" s="1" t="str">
         <v>18hlg1lzF81JB-DJKg36G5SHzOM2zB7Xz</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" s="1" t="str">
         <v>Mathematics and Scientific Computing</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" s="1" t="str">
         <v>Mandi</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="7" xml:space="preserve">
-      <c r="A7" t="str">
+      <c r="A7" s="1" t="str">
         <v>Ekansh Verma</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" s="1" t="str">
         <v>https://www.linkedin.com/in/ekansh-verma-469557228</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="1" t="str">
+        <v>https://www.instagram.com/i_ekanshverma/</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <v>../members/ekansh.webp</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" s="1" t="str">
         <v>1upS_dc_SLM0CsaA__dVnXqApgS4eFKD1</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" s="1" t="str">
         <v>Kullu</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J7" t="str" xml:space="preserve">
+      <c r="K7" s="1" t="str" xml:space="preserve">
         <v xml:space="preserve">Electrical Engineering undergrad at NITH. 
 Interested in Graphic designing &amp; Web designing 
 Photographer &amp; Traveller</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
+      <c r="A8" s="1" t="str">
         <v>Gargi Dhawan</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" s="1" t="str">
         <v>https://www.linkedin.com/in/gargi-dhawan-7706a722a</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="1" t="str">
+        <v>https://www.instagram.com/gargidh1/</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <v>../members/gargi.webp</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" s="1" t="str">
         <v>1HD-obHJOhcS0BYxzv4SRHdRGRnCJ4d-H</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" s="1" t="str">
         <v>Electronics and Communication Engineering</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" s="1" t="str">
         <v>Shimla</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" s="1" t="str">
         <v>Himacha pradesh</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
+      <c r="A9" s="1" t="str">
         <v>Hardik Sachdeva</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="1" t="str">
         <v>https://www.linkedin.com/in/hardik-sachdeva-a69987217</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="1" t="str">
+        <v>https://www.instagram.com/_haardyy_/</v>
+      </c>
+      <c r="F9" s="1" t="str">
         <v>../members/hardik.webp</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" s="1" t="str">
         <v>Mathematics and Scientific Computing</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" s="1" t="str">
         <v>Nainital</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" s="1" t="str">
         <v>Uttarakhand</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" s="1" t="str">
         <v>Pursuing BTech in Mathematics And Computing (2025), Interested in Tech. And Financial Stuff. Travel Freak</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
+      <c r="A10" s="1" t="str">
         <v>Jeevak Sangodkar</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10" s="1" t="str">
         <v>https://www.linkedin.com/in/jeevak-sangodkar-919653228/</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="1" t="str">
+        <v>https://www.instagram.com/jeevaks17/</v>
+      </c>
+      <c r="F10" s="1" t="str">
         <v>../members/jeevak.webp</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" s="1" t="str">
         <v>16_rAwwruLc2BS3XuKMGjF2K70foAL39d</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" s="1" t="str">
         <v>Computer science and Engineering</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" s="1" t="str">
         <v>Nagpur</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" s="1" t="str">
         <v>Maharashtra</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
+      <c r="A11" s="1" t="str">
         <v xml:space="preserve">Kanika Sharma </v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="1" t="str">
         <v>Executive  Member</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="1" t="str">
         <v>https://www.linkedin.com/in/kanika-sharma-aa274b22a</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="1" t="str">
+        <v>https://www.instagram.com/kanika_shh/</v>
+      </c>
+      <c r="F11" s="1" t="str">
         <v>../members/kanika.webp</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" s="1" t="str">
         <v>1cMSLUYaTd_-_d0bWjLBF-VVSiQcmPDaX</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" s="1" t="str">
         <v>First year undergrad at NITH; technology enthusiast</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
+      <c r="A12" s="1" t="str">
         <v>Kuldeep Kumar</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D12" s="1" t="str">
         <v>https://www.linkedin.com/in/kuldeep-kumar-205a9b229/</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12" s="1" t="str">
+        <v>https://www.instagram.com/_.kuldeep_kumar._/</v>
+      </c>
+      <c r="F12" s="1" t="str">
         <v>../members/kuldeep.webp</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" s="1" t="str">
         <v>156x7nF6Vjqlqz0aV1u_krIV2F0B-lvpm</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" s="1" t="str">
         <v>Computer science and Engineering</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" s="1" t="str">
         <v>Solan</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
+      <c r="A13" s="1" t="str">
         <v>Madhukesh Singh</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" s="1" t="str">
         <v>https://www.linkedin.com/in/madhukesh-singh-195618233/</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E13" s="1" t="str">
+        <v>https://www.instagram.com/madhukesh_singh/</v>
+      </c>
+      <c r="F13" s="1" t="str">
         <v>../members/madhukesh.webp</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" s="1" t="str">
         <v>1G1H5v8mdSJ_Us4i1IQtIrSrkYvOBWHWm</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" s="1" t="str">
         <v>Chemical Engineering</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" s="1" t="str">
         <v>Patna</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" s="1" t="str">
         <v>Bihar</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
+      <c r="A14" s="1" t="str">
         <v xml:space="preserve">Manik Singh </v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14" s="1" t="str">
         <v>https://www.linkedin.com/in/manik-singh-021945194/</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E14" s="1" t="str">
+        <v>https://www.instagram.com/maniksingh2002/</v>
+      </c>
+      <c r="F14" s="1" t="str">
         <v>../members/manik.webp</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" s="1" t="str">
         <v>1ijjGG-_dZMlx93qwdHh_MsDrI7vzqgGe</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" s="1" t="str">
         <v>Electronics and Communication Engineering</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
+      <c r="A15" s="1" t="str">
         <v>Mehul Aggarwal</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" s="1" t="str">
         <v>https://www.linkedin.com/in/mehul-aggarwal-47285421b/</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E15" s="1" t="str">
+        <v>https://www.instagram.com/mehul_tp26/</v>
+      </c>
+      <c r="F15" s="1" t="str">
         <v>../members/mehul.webp</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" s="1" t="str">
         <v>1_J6_Pqr7pITVZdau7N3K8iZZXftah1kj</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" s="1" t="str">
         <v>Mathematics and Scientific Computing</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" s="1" t="str">
         <v>Haridwar</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" s="1" t="str">
         <v>Uttarakhand</v>
       </c>
-      <c r="J15" t="str">
+      <c r="K15" s="1" t="str">
         <v>A student at NIT Hamirpur currently pursuing Mathematics and Computing; learning ,trying and testing new technologies and skills everyday.</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
+      <c r="A16" s="1" t="str">
         <v>Navdeep Kaur</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" s="1" t="str">
         <v>https://www.linkedin.com/in/navdeep-kaur-44375022a/</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E16" s="1" t="str">
+        <v>https://www.instagram.com/navikaur_612/</v>
+      </c>
+      <c r="F16" s="1" t="str">
         <v>../members/navdeep.webp</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" s="1" t="str">
         <v>1xKhiNxAbeV8uBDzZRxc6_rxo-opXstOS</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" s="1" t="str">
         <v>Computer science and Engineering</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" s="1" t="str">
         <v>Bilaspur</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J16" t="str">
+      <c r="K16" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
+      <c r="A17" s="1" t="str">
         <v>Shashank Shekhar</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="1" t="str">
         <v>https://www.linkedin.com/in/shashank-shekhar-196786229/</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="1" t="str">
+        <v>https://www.instagram.com/sshekharr28/</v>
+      </c>
+      <c r="F17" s="1" t="str">
         <v>../members/shashank.webp</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" s="1" t="str">
         <v>Mechanical Engineering</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" s="1" t="str">
         <v>Jamui</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" s="1" t="str">
         <v>Bihar</v>
       </c>
-      <c r="J17" t="str">
+      <c r="K17" s="1" t="str">
         <v>Batch 2025</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
+      <c r="A18" s="1" t="str">
         <v>Shariq Verma</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="1" t="str">
         <v>Executive  Member</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18" s="1" t="str">
         <v>https://www.linkedin.com/in/shariq-verma-94a75122a</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E18" s="1" t="str">
+        <v>https://www.instagram.com/shariq_verma/</v>
+      </c>
+      <c r="F18" s="1" t="str">
         <v>../members/Shariq.webp</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" s="1" t="str">
         <v>1KC9wcQ5DgKU31KofULgTIa5VIsbtrttt</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" s="1" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" s="1" t="str">
         <v>Shimla</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J18" t="str">
+      <c r="K18" s="1" t="str">
         <v xml:space="preserve">A Civil Engineering Undergraduate interested in core and currently working on core based technical skills. </v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
+      <c r="A19" s="1" t="str">
         <v>Siya Rana</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19" s="1" t="str">
         <v>https://www.linkedin.com/in/siya-rana-b07639221</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E19" s="1" t="str">
+        <v>https://www.instagram.com/siyarana18_/</v>
+      </c>
+      <c r="F19" s="1" t="str">
         <v>../members/siya.webp</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" s="1" t="str">
         <v>1K4LpZE6yPe1EAsxK6zL7RwGDRhvTk97t</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" s="1" t="str">
         <v>Electronics and Communication Engineering</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J19" t="str">
+      <c r="K19" s="1" t="str">
         <v>First year student at Nit Hamirpur, pursuing Electronics and Communication Engineering.</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="str">
+      <c r="A20" s="1" t="str">
         <v>Swastik Sharma</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="1" t="str">
         <v>Second</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="1" t="str">
         <v>Executive Member</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D20" s="1" t="str">
         <v>https://www.linkedin.com/in/swastkk</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E20" s="1" t="str">
+        <v>https://www.instagram.com/swastik.sharmaa/</v>
+      </c>
+      <c r="F20" s="1" t="str">
         <v>../members/Swastik.webp</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" s="1" t="str">
         <v>15p06FU4eSbaUxpU2A1mq4bD9BS5PxPxu</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" s="1" t="str">
         <v>UNA</v>
       </c>
-      <c r="I20" t="str">
+      <c r="J20" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J20" t="str">
+      <c r="K20" s="1" t="str">
         <v>Electrical Sophomore at NIT Hamirpur currently learning new Web Technologies at Top pace.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K20"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>year</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>description</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" s="1" t="str">
         <v>link</v>
       </c>
-      <c r="E1" t="str">
+      <c r="E1" s="1" t="str">
+        <v>insta</v>
+      </c>
+      <c r="F1" s="1" t="str">
         <v>img</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" s="1" t="str">
         <v>image_link</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" s="1" t="str">
         <v>branch</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" s="1" t="str">
         <v>city</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" s="1" t="str">
         <v>state</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" s="1" t="str">
         <v>about</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>Albert Sharma</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" s="1" t="str">
         <v>https://www.linkedin.com/in/albert-sharma-2016</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E2" s="1" t="str">
+        <v>https://www.instagram.com/b3.berty/</v>
+      </c>
+      <c r="F2" s="1" t="str">
         <v>../members/Albert.webp</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" s="1" t="str">
         <v>1niOjXJKVLFb1ICZ___4pHryOw6ysQt3z</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" s="1" t="str">
         <v>Mathematics and Scientific computing</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" s="1" t="str">
         <v>Bilaspur</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" s="1" t="str">
         <v>Loves to explore the world around Data. Loves to devote time in reading about the Defence forces and the analysis of field decision.</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <v>Deepak Singh</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
         <v>https://www.linkedin.com/in/deepak-singh-a04ba51ba/</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" s="1" t="str">
+        <v>https://www.instagram.com/deepak__9116/</v>
+      </c>
+      <c r="F3" s="1" t="str">
         <v>../members/deepak.jpeg</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" s="1" t="str">
         <v>1LjuDNVhaQmaOaujbP3XWpNtAaXtnAZNo</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" s="1" t="str">
         <v>Computer Science and Engineering</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" s="1" t="str">
         <v>Agra</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" s="1" t="str">
         <v>I am a web developer, a Linux enthusiast, and a piano hobbyist.</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" s="1" t="str">
         <v>Dev Khanduja</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" s="1" t="str">
         <v>https://www.linkedin.com/in/dev-khanduja/</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" s="1" t="str">
+        <v>https://www.instagram.com/dev.khanduja/</v>
+      </c>
+      <c r="F4" s="1" t="str">
         <v>../members/Dev.webp</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" s="1" t="str">
         <v>1Tpnk2k0ZIv73FWy7JeLxcRBjC_Oq7O-f</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" s="1" t="str">
         <v>Mechanical Engineering</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" s="1" t="str">
         <v>Chandigarh</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" s="1" t="str">
         <v>Entrepreneur | Finance Enthusiast | Robotics Aficionado | Psychological Illusionist | Die-Hard Pokémon Fan</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5" s="1" t="str">
         <v>Divyansh Tripathi</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="1" t="str">
         <v>https://www.linkedin.com/in/divyansh-tripathi-4bb66a205</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="1" t="str">
+        <v>https://www.instagram.com/divyanshh007/</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <v>../members/Divyansh.webp</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" s="1" t="str">
         <v>1522oz7z6THBgb0FxF4DmHlyI3YQpviNM</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" s="1" t="str">
         <v>Electronics and Communications Engineering</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" s="1" t="str">
         <v>Greater Noida</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" s="1" t="str">
         <v xml:space="preserve">The Wise Nice guy. ML enthusiast and Geopolitics admirer. </v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <v>Gazal Shyam</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="1" t="str">
+        <v>https://www.instagram.com/_gazalshyam03/</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <v>../members/Gazal.webp</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" s="1" t="str">
         <v>1gYhb-XoUU6OsD2Zrk-eqEUR94UtYotqJ</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" s="1" t="str">
         <v>Computer Science and Engineering</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" s="1" t="str">
         <v>Shimla</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" s="1" t="str">
         <v>Web Dev and ML Enthusiast</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
+      <c r="A7" s="1" t="str">
         <v>Harmanpreet Singh</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="1" t="str">
+        <v>https://www.instagram.com/harmanpreet_013/</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <v>../members/Harmanpreet.webp</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" s="1" t="str">
         <v>18hlg1lzF81JB-DJKg36G5SHzOM2zB7Xz</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" s="1" t="str">
         <v>Computer Science and Engineering Dual</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" s="1" t="str">
         <v>Nalagarh</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" s="1" t="str">
         <v>A computer-science student, web developer, programer, and love to play Hockey.</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
+      <c r="A8" s="1" t="str">
         <v>Harshwardhan Fartale</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="1" t="str">
+        <v>https://www.instagram.com/emharsha_1812</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <v>../members/Harshwardhan.webp</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" s="1" t="str">
         <v>1upS_dc_SLM0CsaA__dVnXqApgS4eFKD1</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" s="1" t="str">
         <v xml:space="preserve">Nagpur </v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" s="1" t="str">
         <v>Maharastra</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" s="1" t="str">
         <v>Electrical Engineer. Web Developer. Designer. Coder. Polymathic</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
+      <c r="A9" s="1" t="str">
         <v>Kartik</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="1" t="str">
         <v>https://www.linkedin.com/in/kartik-576b24205</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="1" t="str">
+        <v>https://www.instagram.com/kart.ik.__/</v>
+      </c>
+      <c r="F9" s="1" t="str">
         <v>../members/Kartik.webp</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" s="1" t="str">
         <v>1HD-obHJOhcS0BYxzv4SRHdRGRnCJ4d-H</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" s="1" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" s="1" t="str">
         <v>Haridwar</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" s="1" t="str">
         <v>Uttrakhand</v>
       </c>
-      <c r="J9" t="str">
-        <v>Digital and graphic art enthusiast. Won&amp;apos;t call myself a nerd but yes I like to write!</v>
+      <c r="K9" s="1" t="str">
+        <v>Digital and graphic art enthusiast. Won't call myself a nerd but yes I like to write!</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
+      <c r="A10" s="1" t="str">
         <v>Kaustubh Verma</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10" s="1" t="str">
         <v>https://www.linkedin.com/in/vermakaustubh28/</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="1" t="str">
+        <v>https://www.instagram.com/kaus._.tubh/</v>
+      </c>
+      <c r="F10" s="1" t="str">
         <v>../members/Kaustubh.webp</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" s="1" t="str">
         <v>16_rAwwruLc2BS3XuKMGjF2K70foAL39d</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" s="1" t="str">
         <v>Mathematics and Scientific computing</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" s="1" t="str">
         <v>Lucknow</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" s="1" t="str">
         <v>Web Developer, Passionate about Machine Learning and why i exist in this world?</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
+      <c r="A11" s="1" t="str">
         <v>Disha Gupta</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="1" t="str">
+        <v>https://www.instagram.com/dg__disha_/</v>
+      </c>
+      <c r="F11" s="1" t="str">
         <v>../members/disha.webp</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" s="1" t="str">
         <v>1cMSLUYaTd_-_d0bWjLBF-VVSiQcmPDaX</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" s="1" t="str">
         <v>Mathematics and Scientific computing</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" s="1" t="str">
         <v>Una</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" s="1" t="str">
         <v>ML enthusiast, Programmer, Developer, Open to learn new technologies</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
+      <c r="A12" s="1" t="str">
         <v>Tanmay Srivastava</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D12" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12" s="1" t="str">
+        <v>https://instagram.com/the_caring_diary?igshid=YmMyMTA2M2Y=</v>
+      </c>
+      <c r="F12" s="1" t="str">
         <v>../members/tanmay.webp</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" s="1" t="str">
         <v>156x7nF6Vjqlqz0aV1u_krIV2F0B-lvpm</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" s="1" t="str">
         <v>Computer Science and Engineering Dual</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" s="1" t="str">
         <v>Ballia</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" s="1" t="str">
         <v>Passionate about coding and desigining softwares for businesses and consumers alike.</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
+      <c r="A13" s="1" t="str">
         <v>Meenakshi</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" s="1" t="str">
         <v>https://www.linkedin.com/in/meenakshi-33b683205</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E13" s="1" t="str">
+        <v>https://www.instagram.com/anana._.p/</v>
+      </c>
+      <c r="F13" s="1" t="str">
         <v>../members/Meenakshi.webp</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" s="1" t="str">
         <v>1G1H5v8mdSJ_Us4i1IQtIrSrkYvOBWHWm</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" s="1" t="str">
         <v>Nalagarh</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" s="1" t="str">
         <v>An intermediate web developer with keen interest in core electrical systems</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
+      <c r="A14" s="1" t="str">
         <v>Noel Kankipati</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14" s="1" t="str">
         <v>https://www.linkedin.com/in/noel-kankipati-444b1a217/</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E14" s="1" t="str">
+        <v>https://www.instagram.com/a_kan_of_nola/</v>
+      </c>
+      <c r="F14" s="1" t="str">
         <v>../members/noel.webp</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" s="1" t="str">
         <v>1ijjGG-_dZMlx93qwdHh_MsDrI7vzqgGe</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" s="1" t="str">
         <v>Mechanical Engineering</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" s="1" t="str">
         <v>Raigarh</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" s="1" t="str">
         <v>Maharastra</v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" s="1" t="str">
         <v>A proud Chef, Core CFD, Automobile, and Aerospace research enthusiast &amp; Photographer.</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
+      <c r="A15" s="1" t="str">
         <v>Shriya Chauhan</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" s="1" t="str">
         <v>https://www.linkedin.com/in/shriya-chauhan-20a19b200</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E15" s="1" t="str">
+        <v>https://instagram.com/girlwithwaves</v>
+      </c>
+      <c r="F15" s="1" t="str">
         <v>../members/shriya.webp</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" s="1" t="str">
         <v>1xKhiNxAbeV8uBDzZRxc6_rxo-opXstOS</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" s="1" t="str">
         <v>Hamirpur</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J15" t="str">
+      <c r="K15" s="1" t="str">
         <v>Batch 2024</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
+      <c r="A16" s="1" t="str">
         <v>Shruti Bhatia</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E16" s="1" t="str">
+        <v>https://instagram.com/the_caring_diary?igshid=YmMyMTA2M2Y=</v>
+      </c>
+      <c r="F16" s="1" t="str">
         <v>../members/Shruti.webp</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" s="1" t="str">
         <v>1KC9wcQ5DgKU31KofULgTIa5VIsbtrttt</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" s="1" t="str">
         <v>Computer Science and Engineering</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" s="1" t="str">
         <v>Solan</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J16" t="str">
+      <c r="K16" s="1" t="str">
         <v>Batch 2024</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
+      <c r="A17" s="1" t="str">
         <v>Sumit Dhiman</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="1" t="str">
         <v>https://www.linkedin.com/in/sumit-dhiman-20bce091</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="1" t="str">
+        <v>https://instagram.com/</v>
+      </c>
+      <c r="F17" s="1" t="str">
         <v>../members/sumit.webp</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" s="1" t="str">
         <v>1K4LpZE6yPe1EAsxK6zL7RwGDRhvTk97t</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" s="1" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" s="1" t="str">
         <v>Hamirpur</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J17" t="str">
+      <c r="K17" s="1" t="str">
         <v>A linux enthusiast, a video editor, Photoshop image manipulator currently pursuing Civil Engineering at National Institute of Technology, Hamirpur(HP)</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
+      <c r="A18" s="1" t="str">
         <v>Vansh Thakur</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18" s="1" t="str">
         <v>https://www.linkedin.com/in/vansh-thakur-b029a4202/</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E18" s="1" t="str">
+        <v>https://www.instagram.com/v.aaaaaa.nsh/</v>
+      </c>
+      <c r="F18" s="1" t="str">
         <v>../members/Vansh.webp</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" s="1" t="str">
         <v>15p06FU4eSbaUxpU2A1mq4bD9BS5PxPxu</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" s="1" t="str">
         <v xml:space="preserve">Himachal Pradesh </v>
       </c>
-      <c r="J18" t="str">
+      <c r="K18" s="1" t="str">
         <v>Hardware geek and an intelligent systems enthusiast</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
+      <c r="A19" s="1" t="str">
         <v>Vanshika Sood</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="1" t="str">
         <v>Third</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="1" t="str">
         <v>Coordinator</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E19" s="1" t="str">
+        <v>https://www.instagram.com/vanshikasood28/</v>
+      </c>
+      <c r="F19" s="1" t="str">
         <v>../members/Vanshika2.webp</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" s="1" t="str">
         <v>1MKW3scd8MOqiME_bAsT0vM9RvYQYeWyR</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" s="1" t="str">
         <v>Computer Science and Engineering</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" s="1" t="str">
         <v>Shimla</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J19" t="str">
+      <c r="K19" s="1" t="str">
         <v>Passionate about graphic design, development and programming.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K19"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>year</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>description</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" s="1" t="str">
         <v>link</v>
       </c>
-      <c r="E1" t="str">
+      <c r="E1" s="1" t="str">
+        <v>insta</v>
+      </c>
+      <c r="F1" s="1" t="str">
         <v>img</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" s="1" t="str">
         <v>image_link</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" s="1" t="str">
         <v>branch</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" s="1" t="str">
         <v>city</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" s="1" t="str">
         <v>state</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" s="1" t="str">
         <v>about</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>Ayushi Sharma</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="1" t="str">
         <v>Secretary</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" s="1" t="str">
         <v>https://www.linkedin.com/in/ayushi-sharma-778657198/</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E2" s="1" t="str">
+        <v>https://www.instagram.com/just._a._potato/</v>
+      </c>
+      <c r="F2" s="1" t="str">
         <v>../members/ayushi.webp</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" s="1" t="str">
         <v>1Tpnk2k0ZIv73FWy7JeLxcRBjC_Oq7O-f</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" s="1" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" s="1" t="str">
         <v>Solan</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" s="1" t="str">
         <v>Passionate about Glaciology and High Mountain Environments.</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <v>Gaurav</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="1" t="str">
         <v>Joint Technical Head</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
         <v>https://www.linkedin.com/in/gaurav-2b5a73195/</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" s="1" t="str">
+        <v>https://www.instagram.com/gauravsml/</v>
+      </c>
+      <c r="F3" s="1" t="str">
         <v>../members/gaurav2.webp</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" s="1" t="str">
         <v>1xKhiNxAbeV8uBDzZRxc6_rxo-opXstOS</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" s="1" t="str">
         <v>Electronics and Communications Engineering</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" s="1" t="str">
         <v>Shimla</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" s="1" t="str">
         <v>Effective Engineering Student committed to learning, developing skills and team contribution. Self-directed and energetic. My fields of interest are software development and Artificial Intelligence/Machine Learning.</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" s="1" t="str">
         <v>Gaurav Pandey</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="1" t="str">
         <v>Vice Chairperson</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" s="1" t="str">
         <v>https://www.linkedin.com/in/gaurav-pandey-412180194/</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" s="1" t="str">
+        <v>https://www.instagram.com/gauravpandey2505/</v>
+      </c>
+      <c r="F4" s="1" t="str">
         <v>../members/gaurav.webp</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" s="1" t="str">
         <v>1niOjXJKVLFb1ICZ___4pHryOw6ysQt3z</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" s="1" t="str">
         <v>Computer Science and Engineering</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" s="1" t="str">
         <v>Bilaspur</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" s="1" t="str">
         <v>Chhattisgarh</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" s="1" t="str">
         <v>A developer by heart and open - source enthusiast eager to develop free and amazing softwares.</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5" s="1" t="str">
         <v>Jai Gupta</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="str">
         <v>Vice Chairperson</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="1" t="str">
         <v>https://www.linkedin.com/in/jai-gupta-8b5238196/</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="1" t="str">
+        <v>https://www.instagram.com/jai_._gupta/</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <v>../members/jai.webp</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" s="1" t="str">
         <v>1522oz7z6THBgb0FxF4DmHlyI3YQpviNM</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" s="1" t="str">
         <v>Mechanical Engineering</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" s="1" t="str">
         <v>Mandi</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" s="1" t="str">
         <v>I am Jai Gupta pre final year undergraduate, enrolled in bachelor of mechanical engineering at National Institute of Technology Hamirpur.</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <v>Kunal Thakur</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="str">
         <v>Marketing Head</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="1" t="str">
         <v>https://www.linkedin.com/in/kunal-thakur-b27823193/</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="1" t="str">
+        <v>https://www.instagram.com/friqxter/</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <v>../members/kunalt.webp</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" s="1" t="str">
         <v>1LjuDNVhaQmaOaujbP3XWpNtAaXtnAZNo</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" s="1" t="str">
         <v>Agra</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" s="1" t="str">
         <v>I have keen interest in 3D modeling softwares and simulation of different mechanisms. Skilled in SOLIDWORKS,Coppelia Sim Robotics,OpenCV, ROS, Gazebo, Lightroom, Computer Vision.</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
+      <c r="A7" s="1" t="str">
         <v>Manvendra Singh Chauhan</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="str">
         <v>Finance Head</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" s="1" t="str">
         <v>https://www.instagram.com/mnvndra/</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="1" t="str">
+        <v>https://www.instagram.com/mnvndra</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <v>../members/manvendra.webp</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" s="1" t="str">
         <v>1gYhb-XoUU6OsD2Zrk-eqEUR94UtYotqJ</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" s="1" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" s="1" t="str">
         <v>Udaipur</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" s="1" t="str">
         <v>Rajasthan</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
+      <c r="A8" s="1" t="str">
         <v>Mayur Kumar</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="1" t="str">
         <v>Chairperson</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" s="1" t="str">
         <v>https://www.linkedin.com/in/mayur-kumar-47a9511a1/</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="1" t="str">
+        <v>https://www.instagram.com/strong10mede/</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <v>../members/mayur.webp</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" s="1" t="str">
         <v>18hlg1lzF81JB-DJKg36G5SHzOM2zB7Xz</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" s="1" t="str">
         <v>Computer Science and Engineering Dual Degree</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" s="1" t="str">
         <v>Patna</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" s="1" t="str">
         <v>Bihar</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" s="1" t="str">
         <v>Have experienced team works and handled financial works for an event plus management of events</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
+      <c r="A9" s="1" t="str">
         <v>Paras Aggarwal</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="1" t="str">
         <v>Joint Secretary</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="1" t="str">
         <v>https://www.linkedin.com/in/parasaggarwal/</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="1" t="str">
+        <v>https://www.instagram.com/arceious/</v>
+      </c>
+      <c r="F9" s="1" t="str">
         <v>../members/paras.webp</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" s="1" t="str">
         <v>1upS_dc_SLM0CsaA__dVnXqApgS4eFKD1</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" s="1" t="str">
         <v>Mechanical Engineering</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" s="1" t="str">
         <v>I am a young Mechanical Engineering enthusiast, interested deeply in learning about the fields of Aerospace, Automobile, Mechatronics, Computer Aided Designing (CAD), Computer Programming and many more. I like to work with CAD a lot. I am good at oration and presentations.</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
+      <c r="A10" s="1" t="str">
         <v>Parth Pant</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="1" t="str">
         <v>Technical Head</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10" s="1" t="str">
         <v>https://www.linkedin.com/in/parth-pant-866bb4189/</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="1" t="str">
+        <v>https://www.instagram.com/pantparth/</v>
+      </c>
+      <c r="F10" s="1" t="str">
         <v>../members/parth.webp</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" s="1" t="str">
         <v>1HD-obHJOhcS0BYxzv4SRHdRGRnCJ4d-H</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" s="1" t="str">
         <v>Electronics and Communications Engineering</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" s="1" t="str">
         <v>Lucknow</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" s="1" t="str">
         <v>I am interested in software engineering and have worked on desktop and web application development. I am constantly looking for new learning opportunities. Currently seeking an entry-level opportunity at an esteemed organization where I can use and enhance my skills and master new technologies.</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
+      <c r="A11" s="1" t="str">
         <v>Pragya Angra</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="1" t="str">
         <v>Joint Design Head</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="1" t="str">
         <v>https://www.linkedin.com/in/pragya-angra-3a87421a9/</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="1" t="str">
+        <v>https://www.instagram.com/</v>
+      </c>
+      <c r="F11" s="1" t="str">
         <v>../members/pragya.webp</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" s="1" t="str">
         <v>1KC9wcQ5DgKU31KofULgTIa5VIsbtrttt</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" s="1" t="str">
         <v>Civil Engineering</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" s="1" t="str">
         <v>Una</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
+      <c r="A12" s="1" t="str">
         <v>Rahul Kumar</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="1" t="str">
         <v>Creative Head</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D12" s="1" t="str">
         <v>https://www.istenith.com/</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12" s="1" t="str">
+        <v>https://www.instagram.com/rahulkumar_rkm_/</v>
+      </c>
+      <c r="F12" s="1" t="str">
         <v>../members/na.webp</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" s="1" t="str">
         <v>16_rAwwruLc2BS3XuKMGjF2K70foAL39d</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" s="1" t="str">
         <v>Lucknow</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
+      <c r="A13" s="1" t="str">
         <v>Suryansh Dwivedi</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="1" t="str">
         <v>Joint Finance Head</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" s="1" t="str">
         <v>https://www.linkedin.com/in/suryansh-dwivedi-9b9975199/</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E13" s="1" t="str">
+        <v>https://www.instagram.com/ansh_of_surya/</v>
+      </c>
+      <c r="F13" s="1" t="str">
         <v>../members/suryansh.webp</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" s="1" t="str">
         <v>1cMSLUYaTd_-_d0bWjLBF-VVSiQcmPDaX</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" s="1" t="str">
         <v>Electronics and Communications Engineering</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" s="1" t="str">
         <v>Hamirpur</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
+      <c r="A14" s="1" t="str">
         <v>Uditee Singh</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="1" t="str">
         <v>Joint PR Head</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14" s="1" t="str">
         <v>https://www.linkedin.com/in/uditee-singh-7619921b0/</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E14" s="1" t="str">
+        <v>https://www.instagram.com/_mois__elle_/</v>
+      </c>
+      <c r="F14" s="1" t="str">
         <v>../members/uditee.webp</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" s="1" t="str">
         <v>1G1H5v8mdSJ_Us4i1IQtIrSrkYvOBWHWm</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" s="1" t="str">
         <v>Electrical Engineering</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
+      <c r="A15" s="1" t="str">
         <v>Utkarsh Rai</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="1" t="str">
         <v>Design Head</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" s="1" t="str">
         <v>https://www.linkedin.com/in/utkarsh-rai-50738b61/</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E15" s="1" t="str">
+        <v>https://www.instagram.com/raiutkarsh09/</v>
+      </c>
+      <c r="F15" s="1" t="str">
         <v>../members/utkarsh.webp</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" s="1" t="str">
         <v>156x7nF6Vjqlqz0aV1u_krIV2F0B-lvpm</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" s="1" t="str">
         <v>Chemical Engineering</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" s="1" t="str">
         <v>Agra</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" s="1" t="str">
         <v>Uttar Pradesh</v>
       </c>
-      <c r="J15" t="str">
+      <c r="K15" s="1" t="str">
         <v>A machine learning enthusiast ,A photographer and a free time video post producer with the backbone of currently pursuing Chemical engineering at National Institute of Technology, Hamirpur(HP). Codes brainstorm me sometimes tho.</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
+      <c r="A16" s="1" t="str">
         <v>Vanshika Thakur</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="1" t="str">
         <v>PR Head</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" s="1" t="str">
         <v>https://www.linkedin.com/in/vanshika-thakur-6a7b4a19a/</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E16" s="1" t="str">
+        <v>https://www.instagram.com/__vanshika__thakur_/</v>
+      </c>
+      <c r="F16" s="1" t="str">
         <v>../members/vanshika.webp</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" s="1" t="str">
         <v>1ijjGG-_dZMlx93qwdHh_MsDrI7vzqgGe</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" s="1" t="str">
         <v>Computer Science and Engineering Dual Degree</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" s="1" t="str">
         <v>Hamirpur</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J16" t="str">
+      <c r="K16" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
+      <c r="A17" s="1" t="str">
         <v>Vasundhra Thakur</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <v>Final</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="1" t="str">
         <v>Joint Secretary</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="1" t="str">
         <v>https://www.linkedin.com/in/vasundhra-thakur-5b9023196/</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="1" t="str">
+        <v>https://www.instagram.com/t.vasundhra/</v>
+      </c>
+      <c r="F17" s="1" t="str">
         <v>../members/vasundhra.webp</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" s="1" t="str">
         <v>1_J6_Pqr7pITVZdau7N3K8iZZXftah1kj</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" s="1" t="str">
         <v>Electronics and Communication Dual Degree</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" s="1" t="str">
         <v>Kangra</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" s="1" t="str">
         <v>Himachal Pradesh</v>
       </c>
-      <c r="J17" t="str">
+      <c r="K17" s="1" t="str">
         <v>Batch 2023</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>